<commit_message>
Add stats for UNSC + add more stats for EMSC + update stats after edition 15 + add playlist editor
</commit_message>
<xml_diff>
--- a/Running Order Stats.xlsx
+++ b/Running Order Stats.xlsx
@@ -407,9 +407,9 @@
   <cols>
     <col min="1" max="1" customWidth="1" width="14"/>
     <col min="2" max="2" customWidth="1" width="11"/>
-    <col min="3" max="3" customWidth="1" width="19"/>
+    <col min="3" max="3" customWidth="1" width="11"/>
     <col min="4" max="4" customWidth="1" width="14"/>
-    <col min="5" max="5" customWidth="1" width="19"/>
+    <col min="5" max="5" customWidth="1" width="13"/>
     <col min="6" max="6" customWidth="1" width="5"/>
     <col min="7" max="7" customWidth="1" width="7"/>
     <col min="8" max="8" customWidth="1" width="6"/>
@@ -486,16 +486,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1004</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="1">
-        <v>111.55555555555556</v>
+        <v>104.2</v>
       </c>
       <c r="D2" s="1">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1">
-        <v>7.111111111111111</v>
+        <v>8.8</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P2" s="1">
         <v>4</v>
@@ -534,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -542,19 +542,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>803</v>
+        <v>919</v>
       </c>
       <c r="C3" s="1">
-        <v>89.22222222222223</v>
+        <v>91.9</v>
       </c>
       <c r="D3" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1">
-        <v>10.444444444444445</v>
+        <v>9.5</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -563,19 +563,19 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
@@ -584,13 +584,13 @@
         <v>7</v>
       </c>
       <c r="P3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="1">
         <v>0</v>
       </c>
       <c r="R3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -598,16 +598,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>632</v>
+        <v>707</v>
       </c>
       <c r="C4" s="1">
-        <v>70.22222222222223</v>
+        <v>70.7</v>
       </c>
       <c r="D4" s="1">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="E4" s="1">
-        <v>16.444444444444443</v>
+        <v>16.4</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -631,22 +631,22 @@
         <v>4</v>
       </c>
       <c r="M4" s="1">
+        <v>7</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>4</v>
+      </c>
+      <c r="P4" s="1">
         <v>6</v>
       </c>
-      <c r="N4" s="1">
-        <v>2</v>
-      </c>
-      <c r="O4" s="1">
-        <v>4</v>
-      </c>
-      <c r="P4" s="1">
-        <v>5</v>
-      </c>
       <c r="Q4" s="1">
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -654,16 +654,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>882</v>
+        <v>980</v>
       </c>
       <c r="C5" s="1">
         <v>98</v>
       </c>
       <c r="D5" s="1">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1">
-        <v>9.666666666666666</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -672,28 +672,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L5" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M5" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="1">
         <v>4</v>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -710,16 +710,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>813</v>
+        <v>885</v>
       </c>
       <c r="C6" s="1">
-        <v>90.33333333333333</v>
+        <v>88.5</v>
       </c>
       <c r="D6" s="1">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="E6" s="1">
-        <v>10.88888888888889</v>
+        <v>11.5</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -743,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="M6" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
@@ -752,13 +752,13 @@
         <v>5</v>
       </c>
       <c r="P6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -766,16 +766,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1038</v>
+        <v>1126</v>
       </c>
       <c r="C7" s="1">
-        <v>115.33333333333333</v>
+        <v>112.6</v>
       </c>
       <c r="D7" s="1">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1">
-        <v>4.222222222222222</v>
+        <v>4.4</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -793,19 +793,19 @@
         <v>6</v>
       </c>
       <c r="K7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7" s="1">
         <v>3</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -822,40 +822,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>766</v>
+        <v>874</v>
       </c>
       <c r="C8" s="1">
-        <v>85.11111111111111</v>
+        <v>87.4</v>
       </c>
       <c r="D8" s="1">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E8" s="1">
-        <v>13.444444444444445</v>
+        <v>12.3</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
@@ -864,13 +864,13 @@
         <v>4</v>
       </c>
       <c r="P8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="1">
         <v>0</v>
       </c>
       <c r="R8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -878,16 +878,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>878</v>
+        <v>959</v>
       </c>
       <c r="C9" s="1">
-        <v>97.55555555555556</v>
+        <v>95.9</v>
       </c>
       <c r="D9" s="1">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1">
-        <v>10.333333333333334</v>
+        <v>10.4</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -908,16 +908,16 @@
         <v>4</v>
       </c>
       <c r="L9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9" s="1">
         <v>5</v>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -934,16 +934,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>802</v>
+        <v>886</v>
       </c>
       <c r="C10" s="1">
-        <v>89.11111111111111</v>
+        <v>88.6</v>
       </c>
       <c r="D10" s="1">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E10" s="1">
-        <v>12.333333333333334</v>
+        <v>12.1</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -961,13 +961,13 @@
         <v>2</v>
       </c>
       <c r="K10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -976,13 +976,13 @@
         <v>5</v>
       </c>
       <c r="P10" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
       </c>
       <c r="R10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -990,16 +990,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>701</v>
+        <v>797</v>
       </c>
       <c r="C11" s="1">
-        <v>77.88888888888889</v>
+        <v>79.7</v>
       </c>
       <c r="D11" s="1">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E11" s="1">
-        <v>14.555555555555555</v>
+        <v>13.5</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1014,22 +1014,22 @@
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P11" s="1">
         <v>4</v>
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1046,16 +1046,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>807</v>
+        <v>866</v>
       </c>
       <c r="C12" s="1">
-        <v>89.66666666666667</v>
+        <v>86.6</v>
       </c>
       <c r="D12" s="1">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="E12" s="1">
-        <v>11.11111111111111</v>
+        <v>12.1</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P12" s="1">
         <v>4</v>
@@ -1094,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -1102,16 +1102,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>723</v>
+        <v>760</v>
       </c>
       <c r="C13" s="1">
-        <v>80.33333333333333</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="E13" s="1">
-        <v>14.88888888888889</v>
+        <v>15.9</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -1138,19 +1138,19 @@
         <v>7</v>
       </c>
       <c r="N13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="1">
         <v>5</v>
       </c>
       <c r="P13" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="1">
         <v>1</v>
       </c>
       <c r="R13" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1158,16 +1158,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>720</v>
+        <v>806</v>
       </c>
       <c r="C14" s="1">
-        <v>80</v>
+        <v>80.6</v>
       </c>
       <c r="D14" s="1">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E14" s="1">
-        <v>13.11111111111111</v>
+        <v>12.5</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1185,19 +1185,19 @@
         <v>1</v>
       </c>
       <c r="K14" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L14" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M14" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P14" s="1">
         <v>6</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1214,16 +1214,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>574</v>
+        <v>634</v>
       </c>
       <c r="C15" s="1">
-        <v>63.77777777777778</v>
+        <v>63.4</v>
       </c>
       <c r="D15" s="1">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="E15" s="1">
-        <v>16.88888888888889</v>
+        <v>17.2</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1247,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="M15" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -1259,10 +1259,10 @@
         <v>4</v>
       </c>
       <c r="Q15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -1270,16 +1270,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>800</v>
+        <v>875</v>
       </c>
       <c r="C16" s="1">
-        <v>88.88888888888889</v>
+        <v>87.5</v>
       </c>
       <c r="D16" s="1">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E16" s="1">
-        <v>11.444444444444445</v>
+        <v>11.8</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1300,16 +1300,16 @@
         <v>5</v>
       </c>
       <c r="L16" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M16" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P16" s="1">
         <v>4</v>
@@ -1318,7 +1318,7 @@
         <v>1</v>
       </c>
       <c r="R16" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -1326,16 +1326,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>668</v>
+        <v>753</v>
       </c>
       <c r="C17" s="1">
-        <v>74.22222222222223</v>
+        <v>75.3</v>
       </c>
       <c r="D17" s="1">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E17" s="1">
-        <v>15.555555555555555</v>
+        <v>14.8</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1353,13 +1353,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M17" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N17" s="1">
         <v>1</v>
@@ -1368,13 +1368,13 @@
         <v>6</v>
       </c>
       <c r="P17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="1">
         <v>1</v>
       </c>
       <c r="R17" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -1382,16 +1382,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>665</v>
+        <v>749</v>
       </c>
       <c r="C18" s="1">
-        <v>73.88888888888889</v>
+        <v>74.9</v>
       </c>
       <c r="D18" s="1">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="E18" s="1">
-        <v>14.666666666666666</v>
+        <v>14.1</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1409,19 +1409,19 @@
         <v>1</v>
       </c>
       <c r="K18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L18" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M18" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
       </c>
       <c r="O18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P18" s="1">
         <v>4</v>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -1438,16 +1438,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>781</v>
+        <v>850</v>
       </c>
       <c r="C19" s="1">
-        <v>86.77777777777777</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E19" s="1">
-        <v>11.666666666666666</v>
+        <v>12.4</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>7</v>
       </c>
       <c r="M19" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
@@ -1480,13 +1480,13 @@
         <v>4</v>
       </c>
       <c r="P19" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="1">
         <v>0</v>
       </c>
       <c r="R19" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -1494,16 +1494,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>639</v>
+        <v>692</v>
       </c>
       <c r="C20" s="1">
-        <v>71</v>
+        <v>69.2</v>
       </c>
       <c r="D20" s="1">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="E20" s="1">
-        <v>15.555555555555555</v>
+        <v>16.3</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P20" s="1">
         <v>5</v>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -1550,16 +1550,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>605</v>
+        <v>681</v>
       </c>
       <c r="C21" s="1">
-        <v>67.22222222222223</v>
+        <v>68.1</v>
       </c>
       <c r="D21" s="1">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E21" s="1">
-        <v>16.88888888888889</v>
+        <v>16.6</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1580,16 +1580,16 @@
         <v>1</v>
       </c>
       <c r="L21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P21" s="1">
         <v>7</v>
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -1606,16 +1606,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>742</v>
+        <v>832</v>
       </c>
       <c r="C22" s="1">
-        <v>82.44444444444444</v>
+        <v>83.2</v>
       </c>
       <c r="D22" s="1">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E22" s="1">
-        <v>12.88888888888889</v>
+        <v>12.1</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1630,31 +1630,31 @@
         <v>1</v>
       </c>
       <c r="J22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L22" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M22" s="1">
+        <v>8</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3</v>
+      </c>
+      <c r="P22" s="1">
         <v>7</v>
       </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>3</v>
-      </c>
-      <c r="P22" s="1">
-        <v>6</v>
-      </c>
       <c r="Q22" s="1">
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
@@ -1662,16 +1662,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>681</v>
+        <v>751</v>
       </c>
       <c r="C23" s="1">
-        <v>75.66666666666667</v>
+        <v>75.1</v>
       </c>
       <c r="D23" s="1">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E23" s="1">
-        <v>14.666666666666666</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>6</v>
       </c>
       <c r="M23" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N23" s="1">
         <v>1</v>
@@ -1704,13 +1704,13 @@
         <v>3</v>
       </c>
       <c r="P23" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q23" s="1">
         <v>0</v>
       </c>
       <c r="R23" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -1718,16 +1718,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>801</v>
+        <v>879</v>
       </c>
       <c r="C24" s="1">
-        <v>89</v>
+        <v>87.9</v>
       </c>
       <c r="D24" s="1">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E24" s="1">
-        <v>11.333333333333334</v>
+        <v>11.5</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1748,10 +1748,10 @@
         <v>3</v>
       </c>
       <c r="L24" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M24" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -1760,13 +1760,13 @@
         <v>5</v>
       </c>
       <c r="P24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q24" s="1">
         <v>0</v>
       </c>
       <c r="R24" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -1774,16 +1774,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>590</v>
+        <v>647</v>
       </c>
       <c r="C25" s="1">
-        <v>65.55555555555556</v>
+        <v>64.7</v>
       </c>
       <c r="D25" s="1">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="E25" s="1">
-        <v>17.22222222222222</v>
+        <v>17.7</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1816,13 +1816,13 @@
         <v>4</v>
       </c>
       <c r="P25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="1">
         <v>1</v>
       </c>
       <c r="R25" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
@@ -1830,16 +1830,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>619</v>
+        <v>698</v>
       </c>
       <c r="C26" s="1">
-        <v>68.77777777777777</v>
+        <v>69.8</v>
       </c>
       <c r="D26" s="1">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E26" s="1">
-        <v>17.666666666666668</v>
+        <v>17.1</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1860,16 +1860,16 @@
         <v>2</v>
       </c>
       <c r="L26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P26" s="1">
         <v>5</v>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1968,25 +1968,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1238</v>
+        <v>1353</v>
       </c>
       <c r="C2" s="1">
-        <v>68.77777777777777</v>
+        <v>67.65</v>
       </c>
       <c r="D2" s="1">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E2" s="1">
-        <v>7.222222222222222</v>
+        <v>7.5</v>
       </c>
       <c r="F2" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1">
-        <v>0.8333333333333334</v>
+        <v>0.85</v>
       </c>
       <c r="I2" s="1">
         <v>4</v>
@@ -2004,10 +2004,10 @@
         <v>7</v>
       </c>
       <c r="N2" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O2" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -2018,25 +2018,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1089</v>
+        <v>1199</v>
       </c>
       <c r="C3" s="1">
-        <v>60.5</v>
+        <v>59.95</v>
       </c>
       <c r="D3" s="1">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="E3" s="1">
-        <v>8.944444444444445</v>
+        <v>9.05</v>
       </c>
       <c r="F3" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.6</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -2054,10 +2054,10 @@
         <v>7</v>
       </c>
       <c r="N3" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O3" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P3" s="1">
         <v>1</v>
@@ -2068,25 +2068,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1183</v>
+        <v>1318</v>
       </c>
       <c r="C4" s="1">
-        <v>65.72222222222223</v>
+        <v>65.9</v>
       </c>
       <c r="D4" s="1">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="E4" s="1">
-        <v>7.777777777777778</v>
+        <v>7.75</v>
       </c>
       <c r="F4" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1">
-        <v>0.7777777777777778</v>
+        <v>0.8</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -2101,13 +2101,13 @@
         <v>5</v>
       </c>
       <c r="M4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N4" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O4" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -2118,25 +2118,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1153</v>
+        <v>1219</v>
       </c>
       <c r="C5" s="1">
-        <v>64.05555555555556</v>
+        <v>60.95</v>
       </c>
       <c r="D5" s="1">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="E5" s="1">
-        <v>8.666666666666666</v>
+        <v>9.25</v>
       </c>
       <c r="F5" s="1">
         <v>13</v>
       </c>
       <c r="G5" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1">
-        <v>0.7222222222222222</v>
+        <v>0.65</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
@@ -2157,10 +2157,10 @@
         <v>9</v>
       </c>
       <c r="O5" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -2168,25 +2168,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1219</v>
+        <v>1361</v>
       </c>
       <c r="C6" s="1">
-        <v>67.72222222222223</v>
+        <v>68.05</v>
       </c>
       <c r="D6" s="1">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E6" s="1">
-        <v>8</v>
+        <v>7.85</v>
       </c>
       <c r="F6" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1">
-        <v>0.7222222222222222</v>
+        <v>0.75</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
@@ -2204,10 +2204,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O6" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -2218,25 +2218,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>996</v>
+        <v>1113</v>
       </c>
       <c r="C7" s="1">
-        <v>55.333333333333336</v>
+        <v>55.65</v>
       </c>
       <c r="D7" s="1">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="E7" s="1">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="F7" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1">
-        <v>0.7222222222222222</v>
+        <v>0.75</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2254,10 +2254,10 @@
         <v>4</v>
       </c>
       <c r="N7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O7" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -2268,28 +2268,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1072</v>
+        <v>1177</v>
       </c>
       <c r="C8" s="1">
-        <v>59.55555555555556</v>
+        <v>58.85</v>
       </c>
       <c r="D8" s="1">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="E8" s="1">
-        <v>8.777777777777779</v>
+        <v>8.75</v>
       </c>
       <c r="F8" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1">
-        <v>0.8888888888888888</v>
+        <v>0.85</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
@@ -2298,19 +2298,19 @@
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N8" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O8" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -2318,46 +2318,46 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>903</v>
+        <v>1065</v>
       </c>
       <c r="C9" s="1">
-        <v>50.166666666666664</v>
+        <v>53.25</v>
       </c>
       <c r="D9" s="1">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E9" s="1">
-        <v>11.555555555555555</v>
+        <v>10.65</v>
       </c>
       <c r="F9" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1">
-        <v>0.4444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N9" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O9" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P9" s="1">
         <v>1</v>
@@ -2368,25 +2368,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>997</v>
+        <v>1067</v>
       </c>
       <c r="C10" s="1">
-        <v>55.388888888888886</v>
+        <v>53.35</v>
       </c>
       <c r="D10" s="1">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="E10" s="1">
-        <v>10.222222222222221</v>
+        <v>10.65</v>
       </c>
       <c r="F10" s="1">
         <v>11</v>
       </c>
       <c r="G10" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.55</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>10</v>
       </c>
       <c r="O10" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -2418,46 +2418,46 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>1090</v>
+        <v>1265</v>
       </c>
       <c r="C11" s="1">
-        <v>60.55555555555556</v>
+        <v>63.25</v>
       </c>
       <c r="D11" s="1">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E11" s="1">
-        <v>8.333333333333334</v>
+        <v>7.75</v>
       </c>
       <c r="F11" s="1">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>10</v>
+      </c>
+      <c r="N11" s="1">
         <v>14</v>
       </c>
-      <c r="G11" s="1">
+      <c r="O11" s="1">
         <v>18</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>2</v>
-      </c>
-      <c r="K11" s="1">
-        <v>2</v>
-      </c>
-      <c r="L11" s="1">
-        <v>4</v>
-      </c>
-      <c r="M11" s="1">
-        <v>8</v>
-      </c>
-      <c r="N11" s="1">
-        <v>12</v>
-      </c>
-      <c r="O11" s="1">
-        <v>16</v>
       </c>
       <c r="P11" s="1">
         <v>2</v>
@@ -2468,46 +2468,46 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>980</v>
+        <v>1077</v>
       </c>
       <c r="C12" s="1">
-        <v>54.44444444444444</v>
+        <v>53.85</v>
       </c>
       <c r="D12" s="1">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="E12" s="1">
-        <v>10.277777777777779</v>
+        <v>10.35</v>
       </c>
       <c r="F12" s="1">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1">
         <v>12</v>
       </c>
-      <c r="G12" s="1">
-        <v>18</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>4</v>
-      </c>
-      <c r="N12" s="1">
-        <v>11</v>
-      </c>
       <c r="O12" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P12" s="1">
         <v>2</v>
@@ -2518,46 +2518,46 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1156</v>
+        <v>1265</v>
       </c>
       <c r="C13" s="1">
-        <v>64.22222222222223</v>
+        <v>63.25</v>
       </c>
       <c r="D13" s="1">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E13" s="1">
-        <v>8.222222222222221</v>
+        <v>8.35</v>
       </c>
       <c r="F13" s="1">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1">
+        <v>8</v>
+      </c>
+      <c r="N13" s="1">
         <v>13</v>
       </c>
-      <c r="G13" s="1">
+      <c r="O13" s="1">
         <v>18</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <v>3</v>
-      </c>
-      <c r="M13" s="1">
-        <v>7</v>
-      </c>
-      <c r="N13" s="1">
-        <v>12</v>
-      </c>
-      <c r="O13" s="1">
-        <v>16</v>
       </c>
       <c r="P13" s="1">
         <v>1</v>
@@ -2568,46 +2568,46 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1029</v>
+        <v>1148</v>
       </c>
       <c r="C14" s="1">
-        <v>57.166666666666664</v>
+        <v>57.4</v>
       </c>
       <c r="D14" s="1">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="E14" s="1">
-        <v>10.277777777777779</v>
+        <v>10.1</v>
       </c>
       <c r="F14" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>4</v>
+      </c>
+      <c r="N14" s="1">
+        <v>9</v>
+      </c>
+      <c r="O14" s="1">
         <v>18</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>2</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2</v>
-      </c>
-      <c r="M14" s="1">
-        <v>4</v>
-      </c>
-      <c r="N14" s="1">
-        <v>7</v>
-      </c>
-      <c r="O14" s="1">
-        <v>16</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -2618,46 +2618,46 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>832</v>
+        <v>967</v>
       </c>
       <c r="C15" s="1">
-        <v>46.22222222222222</v>
+        <v>48.35</v>
       </c>
       <c r="D15" s="1">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="E15" s="1">
-        <v>11.61111111111111</v>
+        <v>11.05</v>
       </c>
       <c r="F15" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G15" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="1">
         <v>1</v>
       </c>
       <c r="L15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O15" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P15" s="1">
         <v>2</v>
@@ -2668,46 +2668,46 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1138</v>
+        <v>1260</v>
       </c>
       <c r="C16" s="1">
-        <v>63.22222222222222</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="E16" s="1">
-        <v>8.666666666666666</v>
+        <v>8.6</v>
       </c>
       <c r="F16" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1">
+        <v>9</v>
+      </c>
+      <c r="N16" s="1">
+        <v>11</v>
+      </c>
+      <c r="O16" s="1">
         <v>18</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1">
-        <v>2</v>
-      </c>
-      <c r="L16" s="1">
-        <v>4</v>
-      </c>
-      <c r="M16" s="1">
-        <v>8</v>
-      </c>
-      <c r="N16" s="1">
-        <v>10</v>
-      </c>
-      <c r="O16" s="1">
-        <v>16</v>
       </c>
       <c r="P16" s="1">
         <v>0</v>
@@ -2718,25 +2718,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1053</v>
+        <v>1188</v>
       </c>
       <c r="C17" s="1">
-        <v>58.5</v>
+        <v>59.4</v>
       </c>
       <c r="D17" s="1">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="E17" s="1">
-        <v>9.88888888888889</v>
+        <v>9.65</v>
       </c>
       <c r="F17" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G17" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H17" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.7</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -2745,19 +2745,19 @@
         <v>2</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O17" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
@@ -3018,25 +3018,25 @@
         <v>-1</v>
       </c>
       <c r="B23" s="1">
-        <v>943</v>
+        <v>1078</v>
       </c>
       <c r="C23" s="1">
-        <v>58.9375</v>
+        <v>59.888888888888886</v>
       </c>
       <c r="D23" s="1">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="E23" s="1">
-        <v>10.3125</v>
+        <v>10</v>
       </c>
       <c r="F23" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H23" s="1">
-        <v>0.625</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
@@ -3045,19 +3045,19 @@
         <v>1</v>
       </c>
       <c r="K23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N23" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O23" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P23" s="1">
         <v>1</v>
@@ -3068,25 +3068,25 @@
         <v>-2</v>
       </c>
       <c r="B24" s="1">
-        <v>1078</v>
+        <v>1200</v>
       </c>
       <c r="C24" s="1">
-        <v>59.888888888888886</v>
+        <v>60</v>
       </c>
       <c r="D24" s="1">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="E24" s="1">
-        <v>9.61111111111111</v>
+        <v>9.45</v>
       </c>
       <c r="F24" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H24" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.65</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -3101,13 +3101,13 @@
         <v>3</v>
       </c>
       <c r="M24" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N24" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O24" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -3118,46 +3118,46 @@
         <v>-3</v>
       </c>
       <c r="B25" s="1">
-        <v>930</v>
+        <v>1065</v>
       </c>
       <c r="C25" s="1">
-        <v>51.666666666666664</v>
+        <v>53.25</v>
       </c>
       <c r="D25" s="1">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="E25" s="1">
-        <v>11.222222222222221</v>
+        <v>10.7</v>
       </c>
       <c r="F25" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H25" s="1">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="1">
         <v>2</v>
       </c>
       <c r="L25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M25" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N25" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O25" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P25" s="1">
         <v>2</v>
@@ -3168,25 +3168,25 @@
         <v>-4</v>
       </c>
       <c r="B26" s="1">
-        <v>1200</v>
+        <v>1319</v>
       </c>
       <c r="C26" s="1">
-        <v>66.66666666666667</v>
+        <v>65.95</v>
       </c>
       <c r="D26" s="1">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="E26" s="1">
-        <v>7.611111111111111</v>
+        <v>7.7</v>
       </c>
       <c r="F26" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G26" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H26" s="1">
-        <v>0.8333333333333334</v>
+        <v>0.85</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -3204,10 +3204,10 @@
         <v>7</v>
       </c>
       <c r="N26" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O26" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
@@ -3218,25 +3218,25 @@
         <v>-5</v>
       </c>
       <c r="B27" s="1">
-        <v>893</v>
+        <v>1002</v>
       </c>
       <c r="C27" s="1">
-        <v>49.611111111111114</v>
+        <v>50.1</v>
       </c>
       <c r="D27" s="1">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E27" s="1">
-        <v>11.444444444444445</v>
+        <v>11.25</v>
       </c>
       <c r="F27" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H27" s="1">
-        <v>0.5555555555555556</v>
+        <v>0.55</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
@@ -3251,13 +3251,13 @@
         <v>1</v>
       </c>
       <c r="M27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N27" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O27" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P27" s="1">
         <v>2</v>
@@ -3268,46 +3268,46 @@
         <v>-6</v>
       </c>
       <c r="B28" s="1">
-        <v>1064</v>
+        <v>1161</v>
       </c>
       <c r="C28" s="1">
-        <v>59.111111111111114</v>
+        <v>58.05</v>
       </c>
       <c r="D28" s="1">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="E28" s="1">
-        <v>9.944444444444445</v>
+        <v>10.05</v>
       </c>
       <c r="F28" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>5</v>
+      </c>
+      <c r="N28" s="1">
+        <v>10</v>
+      </c>
+      <c r="O28" s="1">
         <v>18</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0.6111111111111112</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1</v>
-      </c>
-      <c r="M28" s="1">
-        <v>5</v>
-      </c>
-      <c r="N28" s="1">
-        <v>9</v>
-      </c>
-      <c r="O28" s="1">
-        <v>16</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
@@ -3318,46 +3318,46 @@
         <v>-7</v>
       </c>
       <c r="B29" s="1">
-        <v>1218</v>
+        <v>1393</v>
       </c>
       <c r="C29" s="1">
-        <v>67.66666666666667</v>
+        <v>69.65</v>
       </c>
       <c r="D29" s="1">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E29" s="1">
-        <v>6.555555555555555</v>
+        <v>6.15</v>
       </c>
       <c r="F29" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1">
+        <v>3</v>
+      </c>
+      <c r="L29" s="1">
+        <v>6</v>
+      </c>
+      <c r="M29" s="1">
+        <v>14</v>
+      </c>
+      <c r="N29" s="1">
+        <v>17</v>
+      </c>
+      <c r="O29" s="1">
         <v>18</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="I29" s="1">
-        <v>1</v>
-      </c>
-      <c r="J29" s="1">
-        <v>1</v>
-      </c>
-      <c r="K29" s="1">
-        <v>3</v>
-      </c>
-      <c r="L29" s="1">
-        <v>5</v>
-      </c>
-      <c r="M29" s="1">
-        <v>12</v>
-      </c>
-      <c r="N29" s="1">
-        <v>15</v>
-      </c>
-      <c r="O29" s="1">
-        <v>16</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
@@ -3368,25 +3368,25 @@
         <v>-8</v>
       </c>
       <c r="B30" s="1">
-        <v>871</v>
+        <v>941</v>
       </c>
       <c r="C30" s="1">
-        <v>48.388888888888886</v>
+        <v>47.05</v>
       </c>
       <c r="D30" s="1">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="E30" s="1">
-        <v>10.944444444444445</v>
+        <v>11.3</v>
       </c>
       <c r="F30" s="1">
         <v>11</v>
       </c>
       <c r="G30" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H30" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.55</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -3407,7 +3407,7 @@
         <v>7</v>
       </c>
       <c r="O30" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P30" s="1">
         <v>3</v>
@@ -3418,46 +3418,46 @@
         <v>-9</v>
       </c>
       <c r="B31" s="1">
-        <v>959</v>
+        <v>1121</v>
       </c>
       <c r="C31" s="1">
-        <v>53.27777777777778</v>
+        <v>56.05</v>
       </c>
       <c r="D31" s="1">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E31" s="1">
-        <v>10.444444444444445</v>
+        <v>9.65</v>
       </c>
       <c r="F31" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G31" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H31" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.7</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
       </c>
       <c r="J31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M31" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N31" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O31" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P31" s="1">
         <v>0</v>
@@ -3468,28 +3468,28 @@
         <v>-10</v>
       </c>
       <c r="B32" s="1">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="C32" s="1">
-        <v>56.94444444444444</v>
+        <v>56.5</v>
       </c>
       <c r="D32" s="1">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="E32" s="1">
-        <v>9.944444444444445</v>
+        <v>9.8</v>
       </c>
       <c r="F32" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G32" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H32" s="1">
-        <v>0.7222222222222222</v>
+        <v>0.7</v>
       </c>
       <c r="I32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="1">
         <v>0</v>
@@ -3498,19 +3498,19 @@
         <v>0</v>
       </c>
       <c r="L32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N32" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O32" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -3518,25 +3518,25 @@
         <v>-11</v>
       </c>
       <c r="B33" s="1">
-        <v>939</v>
+        <v>1056</v>
       </c>
       <c r="C33" s="1">
-        <v>52.166666666666664</v>
+        <v>52.8</v>
       </c>
       <c r="D33" s="1">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="E33" s="1">
-        <v>10.666666666666666</v>
+        <v>10.5</v>
       </c>
       <c r="F33" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G33" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H33" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.7</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -3554,10 +3554,10 @@
         <v>2</v>
       </c>
       <c r="N33" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O33" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P33" s="1">
         <v>2</v>
@@ -3568,25 +3568,25 @@
         <v>-12</v>
       </c>
       <c r="B34" s="1">
-        <v>1108</v>
+        <v>1250</v>
       </c>
       <c r="C34" s="1">
-        <v>61.55555555555556</v>
+        <v>62.5</v>
       </c>
       <c r="D34" s="1">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="E34" s="1">
-        <v>9.055555555555555</v>
+        <v>8.8</v>
       </c>
       <c r="F34" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G34" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H34" s="1">
-        <v>0.7222222222222222</v>
+        <v>0.75</v>
       </c>
       <c r="I34" s="1">
         <v>2</v>
@@ -3604,10 +3604,10 @@
         <v>6</v>
       </c>
       <c r="N34" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O34" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P34" s="1">
         <v>1</v>
@@ -3618,25 +3618,25 @@
         <v>-13</v>
       </c>
       <c r="B35" s="1">
-        <v>1077</v>
+        <v>1143</v>
       </c>
       <c r="C35" s="1">
-        <v>59.833333333333336</v>
+        <v>57.15</v>
       </c>
       <c r="D35" s="1">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="E35" s="1">
-        <v>9.444444444444445</v>
+        <v>9.95</v>
       </c>
       <c r="F35" s="1">
         <v>12</v>
       </c>
       <c r="G35" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H35" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.6</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -3657,10 +3657,10 @@
         <v>9</v>
       </c>
       <c r="O35" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -3668,25 +3668,25 @@
         <v>-14</v>
       </c>
       <c r="B36" s="1">
-        <v>1121</v>
+        <v>1256</v>
       </c>
       <c r="C36" s="1">
-        <v>62.27777777777778</v>
+        <v>62.8</v>
       </c>
       <c r="D36" s="1">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="E36" s="1">
-        <v>9</v>
+        <v>8.85</v>
       </c>
       <c r="F36" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G36" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H36" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.65</v>
       </c>
       <c r="I36" s="1">
         <v>1</v>
@@ -3701,13 +3701,13 @@
         <v>3</v>
       </c>
       <c r="M36" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N36" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O36" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>
@@ -3718,46 +3718,46 @@
         <v>-15</v>
       </c>
       <c r="B37" s="1">
-        <v>1083</v>
+        <v>1193</v>
       </c>
       <c r="C37" s="1">
-        <v>60.166666666666664</v>
+        <v>59.65</v>
       </c>
       <c r="D37" s="1">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="E37" s="1">
-        <v>9.11111111111111</v>
+        <v>9.2</v>
       </c>
       <c r="F37" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G37" s="1">
+        <v>20</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I37" s="1">
+        <v>3</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>2</v>
+      </c>
+      <c r="L37" s="1">
+        <v>5</v>
+      </c>
+      <c r="M37" s="1">
+        <v>5</v>
+      </c>
+      <c r="N37" s="1">
+        <v>10</v>
+      </c>
+      <c r="O37" s="1">
         <v>18</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="I37" s="1">
-        <v>3</v>
-      </c>
-      <c r="J37" s="1">
-        <v>0</v>
-      </c>
-      <c r="K37" s="1">
-        <v>2</v>
-      </c>
-      <c r="L37" s="1">
-        <v>5</v>
-      </c>
-      <c r="M37" s="1">
-        <v>5</v>
-      </c>
-      <c r="N37" s="1">
-        <v>9</v>
-      </c>
-      <c r="O37" s="1">
-        <v>16</v>
       </c>
       <c r="P37" s="1">
         <v>2</v>
@@ -3768,25 +3768,25 @@
         <v>-16</v>
       </c>
       <c r="B38" s="1">
-        <v>1180</v>
+        <v>1295</v>
       </c>
       <c r="C38" s="1">
-        <v>65.55555555555556</v>
+        <v>64.75</v>
       </c>
       <c r="D38" s="1">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="E38" s="1">
-        <v>8.61111111111111</v>
+        <v>8.75</v>
       </c>
       <c r="F38" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G38" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H38" s="1">
-        <v>0.6111111111111112</v>
+        <v>0.65</v>
       </c>
       <c r="I38" s="1">
         <v>2</v>
@@ -3804,10 +3804,10 @@
         <v>6</v>
       </c>
       <c r="N38" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O38" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P38" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Update stats to handle a different number of gran finalist + regenerate stats
</commit_message>
<xml_diff>
--- a/Running Order Stats.xlsx
+++ b/Running Order Stats.xlsx
@@ -37,7 +37,7 @@
   <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;ВЯРНО&quot;;&quot;ВЯРНО&quot;;&quot;НЕВЯРНО&quot;"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -70,7 +70,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +409,7 @@
   <cols>
     <col min="1" max="1" customWidth="1" width="14"/>
     <col min="2" max="2" customWidth="1" width="11"/>
-    <col min="3" max="3" customWidth="1" width="19"/>
+    <col min="3" max="3" customWidth="1" width="18"/>
     <col min="4" max="4" customWidth="1" width="14"/>
     <col min="5" max="5" customWidth="1" width="19"/>
     <col min="6" max="6" customWidth="1" width="5"/>
@@ -488,16 +488,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2092</v>
+        <v>2173</v>
       </c>
       <c r="C2" s="1">
-        <v>110.10526315789474</v>
+        <v>108.65</v>
       </c>
       <c r="D2" s="1">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="E2" s="1">
-        <v>7.7894736842105265</v>
+        <v>7.85</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
@@ -515,19 +515,19 @@
         <v>9</v>
       </c>
       <c r="K2" s="1">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
         <v>12</v>
-      </c>
-      <c r="L2" s="1">
-        <v>18</v>
-      </c>
-      <c r="M2" s="1">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>11</v>
       </c>
       <c r="P2" s="1">
         <v>8</v>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -544,16 +544,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1640</v>
+        <v>1710</v>
       </c>
       <c r="C3" s="1">
-        <v>86.3157894736842</v>
+        <v>85.5</v>
       </c>
       <c r="D3" s="1">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E3" s="1">
-        <v>11.105263157894736</v>
+        <v>11.1</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -574,10 +574,10 @@
         <v>9</v>
       </c>
       <c r="L3" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M3" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
@@ -589,10 +589,10 @@
         <v>5</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -600,16 +600,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1468</v>
+        <v>1586</v>
       </c>
       <c r="C4" s="1">
-        <v>77.26315789473684</v>
+        <v>79.3</v>
       </c>
       <c r="D4" s="1">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E4" s="1">
-        <v>14.894736842105264</v>
+        <v>14.3</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -618,22 +618,22 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L4" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M4" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N4" s="1">
         <v>2</v>
@@ -642,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="P4" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -656,16 +656,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1607</v>
+        <v>1699</v>
       </c>
       <c r="C5" s="1">
-        <v>84.57894736842105</v>
+        <v>84.95</v>
       </c>
       <c r="D5" s="1">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="E5" s="1">
-        <v>12.210526315789474</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -683,19 +683,19 @@
         <v>5</v>
       </c>
       <c r="K5" s="1">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1">
+        <v>15</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
         <v>11</v>
-      </c>
-      <c r="L5" s="1">
-        <v>12</v>
-      </c>
-      <c r="M5" s="1">
-        <v>14</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>10</v>
       </c>
       <c r="P5" s="1">
         <v>7</v>
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -712,16 +712,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1692</v>
+        <v>1760</v>
       </c>
       <c r="C6" s="1">
-        <v>89.05263157894737</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="E6" s="1">
-        <v>12.105263157894736</v>
+        <v>12.1</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -742,10 +742,10 @@
         <v>10</v>
       </c>
       <c r="L6" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M6" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
@@ -754,13 +754,13 @@
         <v>5</v>
       </c>
       <c r="P6" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -768,16 +768,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1876</v>
+        <v>1979</v>
       </c>
       <c r="C7" s="1">
-        <v>98.73684210526316</v>
+        <v>98.95</v>
       </c>
       <c r="D7" s="1">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E7" s="1">
-        <v>8.894736842105264</v>
+        <v>8.7</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -792,16 +792,16 @@
         <v>5</v>
       </c>
       <c r="J7" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K7" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M7" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
@@ -810,13 +810,13 @@
         <v>12</v>
       </c>
       <c r="P7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -824,16 +824,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1662</v>
+        <v>1740</v>
       </c>
       <c r="C8" s="1">
-        <v>87.47368421052632</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="E8" s="1">
-        <v>12.368421052631579</v>
+        <v>12.25</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -851,13 +851,13 @@
         <v>7</v>
       </c>
       <c r="K8" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L8" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M8" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
@@ -866,13 +866,13 @@
         <v>8</v>
       </c>
       <c r="P8" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="1">
         <v>0</v>
       </c>
       <c r="R8" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -880,16 +880,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1662</v>
+        <v>1758</v>
       </c>
       <c r="C9" s="1">
-        <v>87.47368421052632</v>
+        <v>87.9</v>
       </c>
       <c r="D9" s="1">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E9" s="1">
-        <v>12.473684210526315</v>
+        <v>12.2</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -907,13 +907,13 @@
         <v>4</v>
       </c>
       <c r="K9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L9" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M9" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
@@ -922,13 +922,13 @@
         <v>10</v>
       </c>
       <c r="P9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q9" s="1">
         <v>1</v>
       </c>
       <c r="R9" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -936,40 +936,40 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1728</v>
+        <v>1848</v>
       </c>
       <c r="C10" s="1">
-        <v>90.94736842105263</v>
+        <v>92.4</v>
       </c>
       <c r="D10" s="1">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E10" s="1">
-        <v>10.578947368421053</v>
+        <v>10.15</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L10" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M10" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -978,13 +978,13 @@
         <v>11</v>
       </c>
       <c r="P10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
       </c>
       <c r="R10" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -992,16 +992,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>1573</v>
+        <v>1637</v>
       </c>
       <c r="C11" s="1">
-        <v>82.78947368421052</v>
+        <v>81.85</v>
       </c>
       <c r="D11" s="1">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="E11" s="1">
-        <v>12.842105263157896</v>
+        <v>12.95</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1022,16 +1022,16 @@
         <v>5</v>
       </c>
       <c r="L11" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M11" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P11" s="1">
         <v>8</v>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -1048,16 +1048,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1554</v>
+        <v>1618</v>
       </c>
       <c r="C12" s="1">
-        <v>81.78947368421052</v>
+        <v>80.9</v>
       </c>
       <c r="D12" s="1">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E12" s="1">
-        <v>12.947368421052632</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1078,16 +1078,16 @@
         <v>7</v>
       </c>
       <c r="L12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M12" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P12" s="1">
         <v>11</v>
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -1104,16 +1104,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1568</v>
+        <v>1616</v>
       </c>
       <c r="C13" s="1">
-        <v>87.11111111111111</v>
+        <v>85.05263157894737</v>
       </c>
       <c r="D13" s="1">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="E13" s="1">
-        <v>13.666666666666666</v>
+        <v>13.947368421052632</v>
       </c>
       <c r="F13" s="1">
         <v>4</v>
@@ -1137,7 +1137,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N13" s="1">
         <v>2</v>
@@ -1146,13 +1146,13 @@
         <v>11</v>
       </c>
       <c r="P13" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="1">
         <v>1</v>
       </c>
       <c r="R13" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -1160,19 +1160,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1459</v>
+        <v>1618</v>
       </c>
       <c r="C14" s="1">
-        <v>76.78947368421052</v>
+        <v>80.9</v>
       </c>
       <c r="D14" s="1">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E14" s="1">
-        <v>13.31578947368421</v>
+        <v>12.7</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -1181,19 +1181,19 @@
         <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M14" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N14" s="1">
         <v>1</v>
@@ -1202,13 +1202,13 @@
         <v>7</v>
       </c>
       <c r="P14" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q14" s="1">
         <v>2</v>
       </c>
       <c r="R14" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -1216,16 +1216,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1365</v>
+        <v>1403</v>
       </c>
       <c r="C15" s="1">
-        <v>71.84210526315789</v>
+        <v>70.15</v>
       </c>
       <c r="D15" s="1">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="E15" s="1">
-        <v>15.68421052631579</v>
+        <v>15.9</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
@@ -1249,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="M15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -1258,13 +1258,13 @@
         <v>9</v>
       </c>
       <c r="P15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q15" s="1">
         <v>1</v>
       </c>
       <c r="R15" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -1272,16 +1272,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1477</v>
+        <v>1543</v>
       </c>
       <c r="C16" s="1">
-        <v>77.73684210526316</v>
+        <v>77.15</v>
       </c>
       <c r="D16" s="1">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="E16" s="1">
-        <v>13.105263157894736</v>
+        <v>13.1</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1302,16 +1302,16 @@
         <v>9</v>
       </c>
       <c r="L16" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N16" s="1">
         <v>3</v>
       </c>
       <c r="O16" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P16" s="1">
         <v>7</v>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="R16" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -1328,16 +1328,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1414</v>
+        <v>1529</v>
       </c>
       <c r="C17" s="1">
-        <v>74.42105263157895</v>
+        <v>76.45</v>
       </c>
       <c r="D17" s="1">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E17" s="1">
-        <v>14.842105263157896</v>
+        <v>14.3</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1352,22 +1352,22 @@
         <v>1</v>
       </c>
       <c r="J17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K17" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L17" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M17" s="1">
+        <v>14</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
         <v>13</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="O17" s="1">
-        <v>12</v>
       </c>
       <c r="P17" s="1">
         <v>6</v>
@@ -1376,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -1384,16 +1384,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1578</v>
+        <v>1681</v>
       </c>
       <c r="C18" s="1">
-        <v>83.05263157894737</v>
+        <v>84.05</v>
       </c>
       <c r="D18" s="1">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="E18" s="1">
-        <v>12.894736842105264</v>
+        <v>12.55</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1411,19 +1411,19 @@
         <v>3</v>
       </c>
       <c r="K18" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L18" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
       </c>
       <c r="O18" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P18" s="1">
         <v>9</v>
@@ -1432,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="R18" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -1440,16 +1440,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1350</v>
+        <v>1402</v>
       </c>
       <c r="C19" s="1">
-        <v>71.05263157894737</v>
+        <v>70.1</v>
       </c>
       <c r="D19" s="1">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="E19" s="1">
-        <v>15.368421052631579</v>
+        <v>15.5</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1473,13 +1473,13 @@
         <v>9</v>
       </c>
       <c r="M19" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N19" s="1">
         <v>2</v>
       </c>
       <c r="O19" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P19" s="1">
         <v>6</v>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="R19" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -1496,16 +1496,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>1466</v>
+        <v>1520</v>
       </c>
       <c r="C20" s="1">
-        <v>77.15789473684211</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="E20" s="1">
-        <v>14.210526315789474</v>
+        <v>14.35</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1529,13 +1529,13 @@
         <v>9</v>
       </c>
       <c r="M20" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P20" s="1">
         <v>12</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -1552,16 +1552,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>1371</v>
+        <v>1402</v>
       </c>
       <c r="C21" s="1">
-        <v>72.15789473684211</v>
+        <v>70.1</v>
       </c>
       <c r="D21" s="1">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="E21" s="1">
-        <v>15.789473684210526</v>
+        <v>16.05</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1594,13 +1594,13 @@
         <v>8</v>
       </c>
       <c r="P21" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
       </c>
       <c r="R21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -1608,16 +1608,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>1664</v>
+        <v>1726</v>
       </c>
       <c r="C22" s="1">
-        <v>87.57894736842105</v>
+        <v>86.3</v>
       </c>
       <c r="D22" s="1">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="E22" s="1">
-        <v>11</v>
+        <v>11.25</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1641,13 +1641,13 @@
         <v>14</v>
       </c>
       <c r="M22" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
       </c>
       <c r="O22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P22" s="1">
         <v>13</v>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -1970,46 +1970,46 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2443</v>
+        <v>2599</v>
       </c>
       <c r="C2" s="1">
-        <v>64.28947368421052</v>
+        <v>64.975</v>
       </c>
       <c r="D2" s="1">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="E2" s="1">
-        <v>8.157894736842104</v>
+        <v>7.9</v>
       </c>
       <c r="F2" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1">
         <v>38</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.8421052631578947</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1">
-        <v>7</v>
-      </c>
-      <c r="M2" s="1">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1">
-        <v>25</v>
-      </c>
-      <c r="O2" s="1">
-        <v>36</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -2020,25 +2020,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2186</v>
+        <v>2311</v>
       </c>
       <c r="C3" s="1">
-        <v>59.08108108108108</v>
+        <v>59.256410256410255</v>
       </c>
       <c r="D3" s="1">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="E3" s="1">
-        <v>9.27027027027027</v>
+        <v>9.128205128205128</v>
       </c>
       <c r="F3" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H3" s="1">
-        <v>0.6486486486486487</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>
@@ -2053,13 +2053,13 @@
         <v>6</v>
       </c>
       <c r="M3" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O3" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P3" s="1">
         <v>2</v>
@@ -2070,25 +2070,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2459</v>
+        <v>2555</v>
       </c>
       <c r="C4" s="1">
-        <v>64.71052631578948</v>
+        <v>63.875</v>
       </c>
       <c r="D4" s="1">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="E4" s="1">
-        <v>8.421052631578947</v>
+        <v>8.475</v>
       </c>
       <c r="F4" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1">
-        <v>0.7631578947368421</v>
+        <v>0.75</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -2106,10 +2106,10 @@
         <v>11</v>
       </c>
       <c r="N4" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -2120,25 +2120,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2277</v>
+        <v>2361</v>
       </c>
       <c r="C5" s="1">
-        <v>59.921052631578945</v>
+        <v>59.025</v>
       </c>
       <c r="D5" s="1">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="E5" s="1">
-        <v>8.868421052631579</v>
+        <v>8.975</v>
       </c>
       <c r="F5" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.675</v>
       </c>
       <c r="I5" s="1">
         <v>6</v>
@@ -2156,13 +2156,13 @@
         <v>12</v>
       </c>
       <c r="N5" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O5" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -2170,25 +2170,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2516</v>
+        <v>2625</v>
       </c>
       <c r="C6" s="1">
-        <v>66.21052631578948</v>
+        <v>65.625</v>
       </c>
       <c r="D6" s="1">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="E6" s="1">
-        <v>8.052631578947368</v>
+        <v>8.1</v>
       </c>
       <c r="F6" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>0.7368421052631579</v>
+        <v>0.75</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
@@ -2206,10 +2206,10 @@
         <v>12</v>
       </c>
       <c r="N6" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O6" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -2220,46 +2220,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2061</v>
+        <v>2256</v>
       </c>
       <c r="C7" s="1">
-        <v>54.23684210526316</v>
+        <v>56.4</v>
       </c>
       <c r="D7" s="1">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="E7" s="1">
-        <v>10.210526315789474</v>
+        <v>9.8</v>
       </c>
       <c r="F7" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1">
-        <v>0.6578947368421053</v>
+        <v>0.675</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M7" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N7" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O7" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P7" s="1">
         <v>3</v>
@@ -2270,49 +2270,49 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2097</v>
+        <v>2200</v>
       </c>
       <c r="C8" s="1">
-        <v>55.18421052631579</v>
+        <v>55</v>
       </c>
       <c r="D8" s="1">
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="E8" s="1">
-        <v>9.710526315789474</v>
+        <v>9.625</v>
       </c>
       <c r="F8" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H8" s="1">
-        <v>0.7105263157894737</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="1">
         <v>2</v>
       </c>
       <c r="J8" s="1">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>9</v>
+      </c>
+      <c r="N8" s="1">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1">
+        <v>36</v>
+      </c>
+      <c r="P8" s="1">
         <v>3</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>5</v>
-      </c>
-      <c r="M8" s="1">
-        <v>8</v>
-      </c>
-      <c r="N8" s="1">
-        <v>19</v>
-      </c>
-      <c r="O8" s="1">
-        <v>34</v>
-      </c>
-      <c r="P8" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -2320,25 +2320,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2353</v>
+        <v>2445</v>
       </c>
       <c r="C9" s="1">
-        <v>61.921052631578945</v>
+        <v>61.125</v>
       </c>
       <c r="D9" s="1">
-        <v>341</v>
+        <v>364</v>
       </c>
       <c r="E9" s="1">
-        <v>8.973684210526315</v>
+        <v>9.1</v>
       </c>
       <c r="F9" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.675</v>
       </c>
       <c r="I9" s="1">
         <v>4</v>
@@ -2356,10 +2356,10 @@
         <v>13</v>
       </c>
       <c r="N9" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O9" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P9" s="1">
         <v>1</v>
@@ -2370,46 +2370,46 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2281</v>
+        <v>2428</v>
       </c>
       <c r="C10" s="1">
-        <v>60.026315789473685</v>
+        <v>60.7</v>
       </c>
       <c r="D10" s="1">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="E10" s="1">
-        <v>9.447368421052632</v>
+        <v>9.225</v>
       </c>
       <c r="F10" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1">
-        <v>0.631578947368421</v>
+        <v>0.65</v>
       </c>
       <c r="I10" s="1">
         <v>4</v>
       </c>
       <c r="J10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
       </c>
       <c r="L10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M10" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N10" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O10" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -2420,25 +2420,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2394</v>
+        <v>2510</v>
       </c>
       <c r="C11" s="1">
-        <v>63</v>
+        <v>62.75</v>
       </c>
       <c r="D11" s="1">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="E11" s="1">
-        <v>8.105263157894736</v>
+        <v>8.125</v>
       </c>
       <c r="F11" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1">
-        <v>0.7368421052631579</v>
+        <v>0.75</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
@@ -2453,13 +2453,13 @@
         <v>9</v>
       </c>
       <c r="M11" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N11" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O11" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P11" s="1">
         <v>3</v>
@@ -2470,25 +2470,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>2212</v>
+        <v>2321</v>
       </c>
       <c r="C12" s="1">
-        <v>58.21052631578947</v>
+        <v>58.025</v>
       </c>
       <c r="D12" s="1">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="E12" s="1">
-        <v>9.473684210526315</v>
+        <v>9.425</v>
       </c>
       <c r="F12" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1">
-        <v>0.7105263157894737</v>
+        <v>0.725</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
@@ -2506,10 +2506,10 @@
         <v>11</v>
       </c>
       <c r="N12" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O12" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P12" s="1">
         <v>3</v>
@@ -2520,25 +2520,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2200</v>
+        <v>2332</v>
       </c>
       <c r="C13" s="1">
-        <v>57.89473684210526</v>
+        <v>58.3</v>
       </c>
       <c r="D13" s="1">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="E13" s="1">
-        <v>9.526315789473685</v>
+        <v>9.35</v>
       </c>
       <c r="F13" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1">
-        <v>0.631578947368421</v>
+        <v>0.65</v>
       </c>
       <c r="I13" s="1">
         <v>1</v>
@@ -2547,19 +2547,19 @@
         <v>2</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N13" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O13" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P13" s="1">
         <v>3</v>
@@ -2570,25 +2570,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>2174</v>
+        <v>2285</v>
       </c>
       <c r="C14" s="1">
-        <v>57.21052631578947</v>
+        <v>57.125</v>
       </c>
       <c r="D14" s="1">
-        <v>376</v>
+        <v>392</v>
       </c>
       <c r="E14" s="1">
-        <v>9.894736842105264</v>
+        <v>9.8</v>
       </c>
       <c r="F14" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H14" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.7</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -2603,13 +2603,13 @@
         <v>5</v>
       </c>
       <c r="M14" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N14" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O14" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -2620,25 +2620,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2066</v>
+        <v>2173</v>
       </c>
       <c r="C15" s="1">
-        <v>54.36842105263158</v>
+        <v>54.325</v>
       </c>
       <c r="D15" s="1">
-        <v>388</v>
+        <v>405</v>
       </c>
       <c r="E15" s="1">
-        <v>10.210526315789474</v>
+        <v>10.125</v>
       </c>
       <c r="F15" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G15" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H15" s="1">
-        <v>0.5789473684210527</v>
+        <v>0.6</v>
       </c>
       <c r="I15" s="1">
         <v>3</v>
@@ -2656,10 +2656,10 @@
         <v>9</v>
       </c>
       <c r="N15" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O15" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P15" s="1">
         <v>5</v>
@@ -3020,25 +3020,25 @@
         <v>-1</v>
       </c>
       <c r="B23" s="1">
-        <v>2139</v>
+        <v>2246</v>
       </c>
       <c r="C23" s="1">
-        <v>59.416666666666664</v>
+        <v>59.10526315789474</v>
       </c>
       <c r="D23" s="1">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="E23" s="1">
-        <v>9.86111111111111</v>
+        <v>9.789473684210526</v>
       </c>
       <c r="F23" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G23" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H23" s="1">
-        <v>0.6388888888888888</v>
+        <v>0.6578947368421053</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
@@ -3056,10 +3056,10 @@
         <v>11</v>
       </c>
       <c r="N23" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O23" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P23" s="1">
         <v>1</v>
@@ -3070,25 +3070,25 @@
         <v>-2</v>
       </c>
       <c r="B24" s="1">
-        <v>2281</v>
+        <v>2392</v>
       </c>
       <c r="C24" s="1">
-        <v>60.026315789473685</v>
+        <v>59.8</v>
       </c>
       <c r="D24" s="1">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="E24" s="1">
-        <v>9.342105263157896</v>
+        <v>9.275</v>
       </c>
       <c r="F24" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H24" s="1">
-        <v>0.7368421052631579</v>
+        <v>0.75</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -3103,13 +3103,13 @@
         <v>3</v>
       </c>
       <c r="M24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N24" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O24" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -3120,25 +3120,25 @@
         <v>-3</v>
       </c>
       <c r="B25" s="1">
-        <v>2037</v>
+        <v>2169</v>
       </c>
       <c r="C25" s="1">
-        <v>53.60526315789474</v>
+        <v>54.225</v>
       </c>
       <c r="D25" s="1">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="E25" s="1">
-        <v>10.368421052631579</v>
+        <v>10.15</v>
       </c>
       <c r="F25" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G25" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H25" s="1">
-        <v>0.5526315789473685</v>
+        <v>0.575</v>
       </c>
       <c r="I25" s="1">
         <v>2</v>
@@ -3147,19 +3147,19 @@
         <v>3</v>
       </c>
       <c r="K25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L25" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M25" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N25" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O25" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P25" s="1">
         <v>4</v>
@@ -3170,25 +3170,25 @@
         <v>-4</v>
       </c>
       <c r="B26" s="1">
-        <v>2310</v>
+        <v>2419</v>
       </c>
       <c r="C26" s="1">
-        <v>62.432432432432435</v>
+        <v>62.02564102564103</v>
       </c>
       <c r="D26" s="1">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="E26" s="1">
-        <v>8.513513513513514</v>
+        <v>8.512820512820513</v>
       </c>
       <c r="F26" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G26" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H26" s="1">
-        <v>0.7837837837837838</v>
+        <v>0.7948717948717948</v>
       </c>
       <c r="I26" s="1">
         <v>2</v>
@@ -3206,10 +3206,10 @@
         <v>12</v>
       </c>
       <c r="N26" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O26" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P26" s="1">
         <v>2</v>
@@ -3220,25 +3220,25 @@
         <v>-5</v>
       </c>
       <c r="B27" s="1">
-        <v>2067</v>
+        <v>2183</v>
       </c>
       <c r="C27" s="1">
-        <v>54.39473684210526</v>
+        <v>54.575</v>
       </c>
       <c r="D27" s="1">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="E27" s="1">
-        <v>10.18421052631579</v>
+        <v>10.1</v>
       </c>
       <c r="F27" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G27" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1">
-        <v>0.6052631578947368</v>
+        <v>0.625</v>
       </c>
       <c r="I27" s="1">
         <v>3</v>
@@ -3253,13 +3253,13 @@
         <v>4</v>
       </c>
       <c r="M27" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N27" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O27" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P27" s="1">
         <v>3</v>
@@ -3270,46 +3270,46 @@
         <v>-6</v>
       </c>
       <c r="B28" s="1">
-        <v>2090</v>
+        <v>2237</v>
       </c>
       <c r="C28" s="1">
-        <v>55</v>
+        <v>55.925</v>
       </c>
       <c r="D28" s="1">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="E28" s="1">
-        <v>10.447368421052632</v>
+        <v>10.175</v>
       </c>
       <c r="F28" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G28" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H28" s="1">
-        <v>0.6052631578947368</v>
+        <v>0.625</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
       </c>
       <c r="J28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" s="1">
         <v>1</v>
       </c>
       <c r="L28" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M28" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N28" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O28" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P28" s="1">
         <v>3</v>
@@ -3320,25 +3320,25 @@
         <v>-7</v>
       </c>
       <c r="B29" s="1">
-        <v>2302</v>
+        <v>2394</v>
       </c>
       <c r="C29" s="1">
-        <v>60.578947368421055</v>
+        <v>59.85</v>
       </c>
       <c r="D29" s="1">
-        <v>323</v>
+        <v>346</v>
       </c>
       <c r="E29" s="1">
-        <v>8.5</v>
+        <v>8.65</v>
       </c>
       <c r="F29" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G29" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H29" s="1">
-        <v>0.6578947368421053</v>
+        <v>0.65</v>
       </c>
       <c r="I29" s="1">
         <v>2</v>
@@ -3356,10 +3356,10 @@
         <v>18</v>
       </c>
       <c r="N29" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O29" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P29" s="1">
         <v>2</v>
@@ -3370,49 +3370,49 @@
         <v>-8</v>
       </c>
       <c r="B30" s="1">
-        <v>2218</v>
+        <v>2321</v>
       </c>
       <c r="C30" s="1">
-        <v>58.36842105263158</v>
+        <v>58.025</v>
       </c>
       <c r="D30" s="1">
-        <v>358</v>
+        <v>374</v>
       </c>
       <c r="E30" s="1">
-        <v>9.421052631578947</v>
+        <v>9.35</v>
       </c>
       <c r="F30" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G30" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H30" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.675</v>
       </c>
       <c r="I30" s="1">
         <v>3</v>
       </c>
       <c r="J30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="1">
         <v>0</v>
       </c>
       <c r="L30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M30" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N30" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O30" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -3420,46 +3420,46 @@
         <v>-9</v>
       </c>
       <c r="B31" s="1">
-        <v>2280</v>
+        <v>2475</v>
       </c>
       <c r="C31" s="1">
-        <v>60</v>
+        <v>61.875</v>
       </c>
       <c r="D31" s="1">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E31" s="1">
-        <v>9.18421052631579</v>
+        <v>8.825</v>
       </c>
       <c r="F31" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G31" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H31" s="1">
-        <v>0.7105263157894737</v>
+        <v>0.725</v>
       </c>
       <c r="I31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" s="1">
         <v>3</v>
       </c>
       <c r="K31" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L31" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M31" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N31" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O31" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P31" s="1">
         <v>0</v>
@@ -3470,25 +3470,25 @@
         <v>-10</v>
       </c>
       <c r="B32" s="1">
-        <v>2138</v>
+        <v>2247</v>
       </c>
       <c r="C32" s="1">
-        <v>56.26315789473684</v>
+        <v>56.175</v>
       </c>
       <c r="D32" s="1">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="E32" s="1">
-        <v>9.736842105263158</v>
+        <v>9.7</v>
       </c>
       <c r="F32" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G32" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H32" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.7</v>
       </c>
       <c r="I32" s="1">
         <v>3</v>
@@ -3506,10 +3506,10 @@
         <v>9</v>
       </c>
       <c r="N32" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O32" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P32" s="1">
         <v>2</v>
@@ -3520,25 +3520,25 @@
         <v>-11</v>
       </c>
       <c r="B33" s="1">
-        <v>2194</v>
+        <v>2278</v>
       </c>
       <c r="C33" s="1">
-        <v>57.73684210526316</v>
+        <v>56.95</v>
       </c>
       <c r="D33" s="1">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="E33" s="1">
-        <v>9.68421052631579</v>
+        <v>9.75</v>
       </c>
       <c r="F33" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G33" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1">
-        <v>0.6842105263157895</v>
+        <v>0.675</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
@@ -3556,13 +3556,13 @@
         <v>8</v>
       </c>
       <c r="N33" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O33" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -3570,25 +3570,25 @@
         <v>-12</v>
       </c>
       <c r="B34" s="1">
-        <v>2412</v>
+        <v>2508</v>
       </c>
       <c r="C34" s="1">
-        <v>63.473684210526315</v>
+        <v>62.7</v>
       </c>
       <c r="D34" s="1">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="E34" s="1">
-        <v>8.631578947368421</v>
+        <v>8.675</v>
       </c>
       <c r="F34" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G34" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H34" s="1">
-        <v>0.7368421052631579</v>
+        <v>0.725</v>
       </c>
       <c r="I34" s="1">
         <v>4</v>
@@ -3606,10 +3606,10 @@
         <v>13</v>
       </c>
       <c r="N34" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O34" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P34" s="1">
         <v>2</v>
@@ -3620,25 +3620,25 @@
         <v>-13</v>
       </c>
       <c r="B35" s="1">
-        <v>2188</v>
+        <v>2313</v>
       </c>
       <c r="C35" s="1">
-        <v>57.578947368421055</v>
+        <v>57.825</v>
       </c>
       <c r="D35" s="1">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="E35" s="1">
-        <v>9.552631578947368</v>
+        <v>9.4</v>
       </c>
       <c r="F35" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1">
-        <v>0.631578947368421</v>
+        <v>0.65</v>
       </c>
       <c r="I35" s="1">
         <v>1</v>
@@ -3653,13 +3653,13 @@
         <v>9</v>
       </c>
       <c r="M35" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N35" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O35" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P35" s="1">
         <v>3</v>
@@ -3670,46 +3670,46 @@
         <v>-14</v>
       </c>
       <c r="B36" s="1">
-        <v>2402</v>
+        <v>2558</v>
       </c>
       <c r="C36" s="1">
-        <v>63.21052631578947</v>
+        <v>63.95</v>
       </c>
       <c r="D36" s="1">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="E36" s="1">
-        <v>8.68421052631579</v>
+        <v>8.4</v>
       </c>
       <c r="F36" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G36" s="1">
+        <v>40</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.675</v>
+      </c>
+      <c r="I36" s="1">
+        <v>5</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1">
+        <v>8</v>
+      </c>
+      <c r="M36" s="1">
+        <v>13</v>
+      </c>
+      <c r="N36" s="1">
+        <v>26</v>
+      </c>
+      <c r="O36" s="1">
         <v>38</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.6578947368421053</v>
-      </c>
-      <c r="I36" s="1">
-        <v>4</v>
-      </c>
-      <c r="J36" s="1">
-        <v>2</v>
-      </c>
-      <c r="K36" s="1">
-        <v>1</v>
-      </c>
-      <c r="L36" s="1">
-        <v>7</v>
-      </c>
-      <c r="M36" s="1">
-        <v>11</v>
-      </c>
-      <c r="N36" s="1">
-        <v>24</v>
-      </c>
-      <c r="O36" s="1">
-        <v>36</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Update the stats to the edition 23
</commit_message>
<xml_diff>
--- a/Running Order Stats.xlsx
+++ b/Running Order Stats.xlsx
@@ -37,7 +37,7 @@
   <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;ВЯРНО&quot;;&quot;ВЯРНО&quot;;&quot;НЕВЯРНО&quot;"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -70,7 +70,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +409,7 @@
   <cols>
     <col min="1" max="1" customWidth="1" width="14"/>
     <col min="2" max="2" customWidth="1" width="11"/>
-    <col min="3" max="3" customWidth="1" width="18"/>
+    <col min="3" max="3" customWidth="1" width="19"/>
     <col min="4" max="4" customWidth="1" width="14"/>
     <col min="5" max="5" customWidth="1" width="19"/>
     <col min="6" max="6" customWidth="1" width="5"/>
@@ -488,19 +488,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2173</v>
+        <v>2423</v>
       </c>
       <c r="C2" s="1">
-        <v>108.65</v>
+        <v>110.13636363636364</v>
       </c>
       <c r="D2" s="1">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E2" s="1">
-        <v>7.85</v>
+        <v>7.363636363636363</v>
       </c>
       <c r="F2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -509,19 +509,19 @@
         <v>3</v>
       </c>
       <c r="I2" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M2" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
@@ -530,13 +530,13 @@
         <v>12</v>
       </c>
       <c r="P2" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="1">
         <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -544,19 +544,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1710</v>
+        <v>1974</v>
       </c>
       <c r="C3" s="1">
-        <v>85.5</v>
+        <v>89.72727272727273</v>
       </c>
       <c r="D3" s="1">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E3" s="1">
-        <v>11.1</v>
+        <v>10.363636363636363</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -565,34 +565,34 @@
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K3" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M3" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P3" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
       </c>
       <c r="R3" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -600,16 +600,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1586</v>
+        <v>1772</v>
       </c>
       <c r="C4" s="1">
-        <v>79.3</v>
+        <v>80.54545454545455</v>
       </c>
       <c r="D4" s="1">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="E4" s="1">
-        <v>14.3</v>
+        <v>13.818181818181818</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -618,22 +618,22 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L4" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M4" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N4" s="1">
         <v>2</v>
@@ -642,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="P4" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -656,16 +656,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1699</v>
+        <v>1798</v>
       </c>
       <c r="C5" s="1">
-        <v>84.95</v>
+        <v>81.72727272727273</v>
       </c>
       <c r="D5" s="1">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="E5" s="1">
-        <v>12</v>
+        <v>12.681818181818182</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -689,22 +689,22 @@
         <v>13</v>
       </c>
       <c r="M5" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P5" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
       <c r="R5" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -712,16 +712,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1760</v>
+        <v>1894</v>
       </c>
       <c r="C6" s="1">
-        <v>88</v>
+        <v>86.0909090909091</v>
       </c>
       <c r="D6" s="1">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="E6" s="1">
-        <v>12.1</v>
+        <v>12.363636363636363</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -739,13 +739,13 @@
         <v>5</v>
       </c>
       <c r="K6" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L6" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M6" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
@@ -754,13 +754,13 @@
         <v>5</v>
       </c>
       <c r="P6" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -768,16 +768,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1979</v>
+        <v>2155</v>
       </c>
       <c r="C7" s="1">
-        <v>98.95</v>
+        <v>97.95454545454545</v>
       </c>
       <c r="D7" s="1">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="E7" s="1">
-        <v>8.7</v>
+        <v>8.590909090909092</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -795,19 +795,19 @@
         <v>9</v>
       </c>
       <c r="K7" s="1">
+        <v>16</v>
+      </c>
+      <c r="L7" s="1">
+        <v>18</v>
+      </c>
+      <c r="M7" s="1">
+        <v>19</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
         <v>14</v>
-      </c>
-      <c r="L7" s="1">
-        <v>16</v>
-      </c>
-      <c r="M7" s="1">
-        <v>17</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>12</v>
       </c>
       <c r="P7" s="1">
         <v>8</v>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -824,16 +824,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1740</v>
+        <v>1868</v>
       </c>
       <c r="C8" s="1">
-        <v>87</v>
+        <v>84.9090909090909</v>
       </c>
       <c r="D8" s="1">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="E8" s="1">
-        <v>12.25</v>
+        <v>12.318181818181818</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -851,19 +851,19 @@
         <v>7</v>
       </c>
       <c r="K8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M8" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P8" s="1">
         <v>12</v>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -880,16 +880,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1758</v>
+        <v>1917</v>
       </c>
       <c r="C9" s="1">
-        <v>87.9</v>
+        <v>87.13636363636364</v>
       </c>
       <c r="D9" s="1">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="E9" s="1">
-        <v>12.2</v>
+        <v>12.227272727272727</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -898,28 +898,28 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L9" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M9" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P9" s="1">
         <v>9</v>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="R9" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -936,16 +936,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1848</v>
+        <v>1993</v>
       </c>
       <c r="C10" s="1">
-        <v>92.4</v>
+        <v>90.5909090909091</v>
       </c>
       <c r="D10" s="1">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="E10" s="1">
-        <v>10.15</v>
+        <v>10.227272727272727</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -960,16 +960,16 @@
         <v>3</v>
       </c>
       <c r="J10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K10" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L10" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -978,13 +978,13 @@
         <v>11</v>
       </c>
       <c r="P10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
       </c>
       <c r="R10" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -992,16 +992,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>1637</v>
+        <v>1781</v>
       </c>
       <c r="C11" s="1">
-        <v>81.85</v>
+        <v>80.95454545454545</v>
       </c>
       <c r="D11" s="1">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="E11" s="1">
-        <v>12.95</v>
+        <v>12.863636363636363</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1019,28 +1019,28 @@
         <v>5</v>
       </c>
       <c r="K11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L11" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M11" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q11" s="1">
         <v>1</v>
       </c>
       <c r="R11" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -1048,16 +1048,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1618</v>
+        <v>1750</v>
       </c>
       <c r="C12" s="1">
-        <v>80.9</v>
+        <v>79.54545454545455</v>
       </c>
       <c r="D12" s="1">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="E12" s="1">
-        <v>13</v>
+        <v>13.181818181818182</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1078,10 +1078,10 @@
         <v>7</v>
       </c>
       <c r="L12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M12" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
@@ -1090,13 +1090,13 @@
         <v>8</v>
       </c>
       <c r="P12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -1104,16 +1104,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1616</v>
+        <v>1753</v>
       </c>
       <c r="C13" s="1">
-        <v>85.05263157894737</v>
+        <v>83.47619047619048</v>
       </c>
       <c r="D13" s="1">
-        <v>265</v>
+        <v>294</v>
       </c>
       <c r="E13" s="1">
-        <v>13.947368421052632</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1">
         <v>4</v>
@@ -1131,13 +1131,13 @@
         <v>5</v>
       </c>
       <c r="K13" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L13" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M13" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N13" s="1">
         <v>2</v>
@@ -1146,13 +1146,13 @@
         <v>11</v>
       </c>
       <c r="P13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q13" s="1">
         <v>1</v>
       </c>
       <c r="R13" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -1160,16 +1160,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1618</v>
+        <v>1693</v>
       </c>
       <c r="C14" s="1">
-        <v>80.9</v>
+        <v>76.95454545454545</v>
       </c>
       <c r="D14" s="1">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="E14" s="1">
-        <v>12.7</v>
+        <v>13.5</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1193,22 +1193,22 @@
         <v>13</v>
       </c>
       <c r="M14" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N14" s="1">
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q14" s="1">
         <v>2</v>
       </c>
       <c r="R14" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
@@ -1216,16 +1216,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1403</v>
+        <v>1584</v>
       </c>
       <c r="C15" s="1">
-        <v>70.15</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="E15" s="1">
-        <v>15.9</v>
+        <v>15.409090909090908</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
@@ -1240,16 +1240,16 @@
         <v>3</v>
       </c>
       <c r="J15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L15" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M15" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -1258,13 +1258,13 @@
         <v>9</v>
       </c>
       <c r="P15" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="1">
         <v>1</v>
       </c>
       <c r="R15" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
@@ -1272,16 +1272,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1543</v>
+        <v>1659</v>
       </c>
       <c r="C16" s="1">
-        <v>77.15</v>
+        <v>75.4090909090909</v>
       </c>
       <c r="D16" s="1">
-        <v>262</v>
+        <v>298</v>
       </c>
       <c r="E16" s="1">
-        <v>13.1</v>
+        <v>13.545454545454545</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1302,10 +1302,10 @@
         <v>9</v>
       </c>
       <c r="L16" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N16" s="1">
         <v>3</v>
@@ -1314,13 +1314,13 @@
         <v>11</v>
       </c>
       <c r="P16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q16" s="1">
         <v>2</v>
       </c>
       <c r="R16" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
@@ -1328,16 +1328,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1529</v>
+        <v>1629</v>
       </c>
       <c r="C17" s="1">
-        <v>76.45</v>
+        <v>74.04545454545455</v>
       </c>
       <c r="D17" s="1">
-        <v>286</v>
+        <v>319</v>
       </c>
       <c r="E17" s="1">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1355,28 +1355,28 @@
         <v>4</v>
       </c>
       <c r="K17" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L17" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M17" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" s="1">
         <v>13</v>
       </c>
       <c r="P17" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q17" s="1">
         <v>1</v>
       </c>
       <c r="R17" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
@@ -1384,16 +1384,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1681</v>
+        <v>1840</v>
       </c>
       <c r="C18" s="1">
-        <v>84.05</v>
+        <v>83.63636363636364</v>
       </c>
       <c r="D18" s="1">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="E18" s="1">
-        <v>12.55</v>
+        <v>12.454545454545455</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1414,25 +1414,25 @@
         <v>9</v>
       </c>
       <c r="L18" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M18" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
       </c>
       <c r="O18" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P18" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q18" s="1">
         <v>4</v>
       </c>
       <c r="R18" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -1440,16 +1440,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1402</v>
+        <v>1563</v>
       </c>
       <c r="C19" s="1">
-        <v>70.1</v>
+        <v>71.04545454545455</v>
       </c>
       <c r="D19" s="1">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="E19" s="1">
-        <v>15.5</v>
+        <v>15.090909090909092</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1467,28 +1467,28 @@
         <v>2</v>
       </c>
       <c r="K19" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L19" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M19" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N19" s="1">
         <v>2</v>
       </c>
       <c r="O19" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P19" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q19" s="1">
         <v>1</v>
       </c>
       <c r="R19" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -1496,16 +1496,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>1520</v>
+        <v>1599</v>
       </c>
       <c r="C20" s="1">
-        <v>76</v>
+        <v>72.68181818181819</v>
       </c>
       <c r="D20" s="1">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="E20" s="1">
-        <v>14.35</v>
+        <v>15.045454545454545</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1529,13 +1529,13 @@
         <v>9</v>
       </c>
       <c r="M20" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P20" s="1">
         <v>12</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -1552,16 +1552,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>1402</v>
+        <v>1501</v>
       </c>
       <c r="C21" s="1">
-        <v>70.1</v>
+        <v>68.22727272727273</v>
       </c>
       <c r="D21" s="1">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="E21" s="1">
-        <v>16.05</v>
+        <v>16.363636363636363</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1585,13 +1585,13 @@
         <v>10</v>
       </c>
       <c r="M21" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N21" s="1">
         <v>1</v>
       </c>
       <c r="O21" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P21" s="1">
         <v>12</v>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
@@ -1608,16 +1608,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>1726</v>
+        <v>1906</v>
       </c>
       <c r="C22" s="1">
-        <v>86.3</v>
+        <v>86.63636363636364</v>
       </c>
       <c r="D22" s="1">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="E22" s="1">
-        <v>11.25</v>
+        <v>10.954545454545455</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1635,28 +1635,28 @@
         <v>5</v>
       </c>
       <c r="K22" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L22" s="1">
+        <v>16</v>
+      </c>
+      <c r="M22" s="1">
+        <v>20</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>8</v>
+      </c>
+      <c r="P22" s="1">
         <v>14</v>
       </c>
-      <c r="M22" s="1">
-        <v>18</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>7</v>
-      </c>
-      <c r="P22" s="1">
-        <v>13</v>
-      </c>
       <c r="Q22" s="1">
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -1664,13 +1664,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1395</v>
+        <v>1520</v>
       </c>
       <c r="C23" s="1">
-        <v>73.42105263157895</v>
+        <v>72.38095238095238</v>
       </c>
       <c r="D23" s="1">
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="E23" s="1">
         <v>15</v>
@@ -1694,16 +1694,16 @@
         <v>3</v>
       </c>
       <c r="L23" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M23" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N23" s="1">
         <v>1</v>
       </c>
       <c r="O23" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P23" s="1">
         <v>13</v>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
@@ -1720,46 +1720,46 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1710</v>
+        <v>1918</v>
       </c>
       <c r="C24" s="1">
-        <v>90</v>
+        <v>91.33333333333333</v>
       </c>
       <c r="D24" s="1">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="E24" s="1">
-        <v>11.31578947368421</v>
+        <v>10.857142857142858</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
       </c>
       <c r="I24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L24" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M24" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
       </c>
       <c r="O24" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P24" s="1">
         <v>8</v>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
@@ -1776,55 +1776,55 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>1373</v>
+        <v>1545</v>
       </c>
       <c r="C25" s="1">
-        <v>72.26315789473684</v>
+        <v>73.57142857142857</v>
       </c>
       <c r="D25" s="1">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="E25" s="1">
-        <v>15.31578947368421</v>
+        <v>15.095238095238095</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L25" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M25" s="1">
+        <v>14</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1">
+        <v>7</v>
+      </c>
+      <c r="P25" s="1">
         <v>13</v>
       </c>
-      <c r="N25" s="1">
-        <v>1</v>
-      </c>
-      <c r="O25" s="1">
-        <v>6</v>
-      </c>
-      <c r="P25" s="1">
-        <v>12</v>
-      </c>
       <c r="Q25" s="1">
         <v>1</v>
       </c>
       <c r="R25" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
@@ -1832,16 +1832,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>1472</v>
+        <v>1575</v>
       </c>
       <c r="C26" s="1">
-        <v>77.47368421052632</v>
+        <v>75</v>
       </c>
       <c r="D26" s="1">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="E26" s="1">
-        <v>14.68421052631579</v>
+        <v>14.952380952380953</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1862,16 +1862,16 @@
         <v>6</v>
       </c>
       <c r="L26" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M26" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P26" s="1">
         <v>8</v>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1899,7 @@
   <cols>
     <col min="1" max="1" customWidth="1" width="14"/>
     <col min="2" max="2" customWidth="1" width="11"/>
-    <col min="3" max="3" customWidth="1" width="19"/>
+    <col min="3" max="3" customWidth="1" width="18"/>
     <col min="4" max="4" customWidth="1" width="14"/>
     <col min="5" max="5" customWidth="1" width="19"/>
     <col min="6" max="6" customWidth="1" width="19"/>
@@ -1970,25 +1970,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2599</v>
+        <v>2861</v>
       </c>
       <c r="C2" s="1">
-        <v>64.975</v>
+        <v>65.02272727272727</v>
       </c>
       <c r="D2" s="1">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="E2" s="1">
-        <v>7.9</v>
+        <v>7.840909090909091</v>
       </c>
       <c r="F2" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1">
-        <v>0.85</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="I2" s="1">
         <v>5</v>
@@ -2006,10 +2006,10 @@
         <v>13</v>
       </c>
       <c r="N2" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -2020,46 +2020,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2311</v>
+        <v>2614</v>
       </c>
       <c r="C3" s="1">
-        <v>59.256410256410255</v>
+        <v>60.7906976744186</v>
       </c>
       <c r="D3" s="1">
-        <v>356</v>
+        <v>379</v>
       </c>
       <c r="E3" s="1">
-        <v>9.128205128205128</v>
+        <v>8.813953488372093</v>
       </c>
       <c r="F3" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.6976744186046512</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1">
         <v>3</v>
       </c>
       <c r="L3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M3" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N3" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P3" s="1">
         <v>2</v>
@@ -2070,46 +2070,46 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2555</v>
+        <v>2757</v>
       </c>
       <c r="C4" s="1">
-        <v>63.875</v>
+        <v>62.65909090909091</v>
       </c>
       <c r="D4" s="1">
-        <v>339</v>
+        <v>381</v>
       </c>
       <c r="E4" s="1">
-        <v>8.475</v>
+        <v>8.659090909090908</v>
       </c>
       <c r="F4" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>8</v>
+      </c>
+      <c r="M4" s="1">
+        <v>12</v>
+      </c>
+      <c r="N4" s="1">
+        <v>29</v>
+      </c>
+      <c r="O4" s="1">
         <v>40</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2</v>
-      </c>
-      <c r="L4" s="1">
-        <v>7</v>
-      </c>
-      <c r="M4" s="1">
-        <v>11</v>
-      </c>
-      <c r="N4" s="1">
-        <v>28</v>
-      </c>
-      <c r="O4" s="1">
-        <v>36</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -2120,25 +2120,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2361</v>
+        <v>2619</v>
       </c>
       <c r="C5" s="1">
-        <v>59.025</v>
+        <v>59.52272727272727</v>
       </c>
       <c r="D5" s="1">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="E5" s="1">
-        <v>8.975</v>
+        <v>8.818181818181818</v>
       </c>
       <c r="F5" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H5" s="1">
-        <v>0.675</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="I5" s="1">
         <v>6</v>
@@ -2147,19 +2147,19 @@
         <v>1</v>
       </c>
       <c r="K5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L5" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M5" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N5" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O5" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P5" s="1">
         <v>5</v>
@@ -2170,28 +2170,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2625</v>
+        <v>2828</v>
       </c>
       <c r="C6" s="1">
-        <v>65.625</v>
+        <v>64.27272727272727</v>
       </c>
       <c r="D6" s="1">
-        <v>324</v>
+        <v>362</v>
       </c>
       <c r="E6" s="1">
-        <v>8.1</v>
+        <v>8.227272727272727</v>
       </c>
       <c r="F6" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1">
         <v>0.75</v>
       </c>
       <c r="I6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1">
         <v>5</v>
@@ -2200,19 +2200,19 @@
         <v>2</v>
       </c>
       <c r="L6" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M6" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N6" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O6" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2220,28 +2220,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2256</v>
+        <v>2475</v>
       </c>
       <c r="C7" s="1">
-        <v>56.4</v>
+        <v>57.55813953488372</v>
       </c>
       <c r="D7" s="1">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="E7" s="1">
-        <v>9.8</v>
+        <v>9.581395348837209</v>
       </c>
       <c r="F7" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1">
-        <v>0.675</v>
+        <v>0.6744186046511628</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
@@ -2250,16 +2250,16 @@
         <v>5</v>
       </c>
       <c r="L7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M7" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N7" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O7" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P7" s="1">
         <v>3</v>
@@ -2270,25 +2270,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2200</v>
+        <v>2395</v>
       </c>
       <c r="C8" s="1">
-        <v>55</v>
+        <v>55.69767441860465</v>
       </c>
       <c r="D8" s="1">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="E8" s="1">
-        <v>9.625</v>
+        <v>9.44186046511628</v>
       </c>
       <c r="F8" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1">
-        <v>0.7</v>
+        <v>0.7209302325581395</v>
       </c>
       <c r="I8" s="1">
         <v>2</v>
@@ -2303,13 +2303,13 @@
         <v>6</v>
       </c>
       <c r="M8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O8" s="1">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="P8" s="1">
         <v>3</v>
@@ -2320,25 +2320,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2445</v>
+        <v>2754</v>
       </c>
       <c r="C9" s="1">
-        <v>61.125</v>
+        <v>62.59090909090909</v>
       </c>
       <c r="D9" s="1">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="E9" s="1">
-        <v>9.1</v>
+        <v>8.818181818181818</v>
       </c>
       <c r="F9" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1">
-        <v>0.675</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="I9" s="1">
         <v>4</v>
@@ -2347,19 +2347,19 @@
         <v>1</v>
       </c>
       <c r="K9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L9" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M9" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N9" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O9" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P9" s="1">
         <v>1</v>
@@ -2370,25 +2370,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2428</v>
+        <v>2595</v>
       </c>
       <c r="C10" s="1">
-        <v>60.7</v>
+        <v>58.97727272727273</v>
       </c>
       <c r="D10" s="1">
-        <v>369</v>
+        <v>413</v>
       </c>
       <c r="E10" s="1">
-        <v>9.225</v>
+        <v>9.386363636363637</v>
       </c>
       <c r="F10" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1">
-        <v>0.65</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="I10" s="1">
         <v>4</v>
@@ -2397,19 +2397,19 @@
         <v>3</v>
       </c>
       <c r="K10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M10" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N10" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O10" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -2420,25 +2420,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2510</v>
+        <v>2744</v>
       </c>
       <c r="C11" s="1">
-        <v>62.75</v>
+        <v>62.36363636363637</v>
       </c>
       <c r="D11" s="1">
-        <v>325</v>
+        <v>358</v>
       </c>
       <c r="E11" s="1">
-        <v>8.125</v>
+        <v>8.136363636363637</v>
       </c>
       <c r="F11" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1">
-        <v>0.75</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
@@ -2453,13 +2453,13 @@
         <v>9</v>
       </c>
       <c r="M11" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N11" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O11" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P11" s="1">
         <v>3</v>
@@ -2470,25 +2470,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>2321</v>
+        <v>2484</v>
       </c>
       <c r="C12" s="1">
-        <v>58.025</v>
+        <v>56.45454545454545</v>
       </c>
       <c r="D12" s="1">
-        <v>377</v>
+        <v>421</v>
       </c>
       <c r="E12" s="1">
-        <v>9.425</v>
+        <v>9.568181818181818</v>
       </c>
       <c r="F12" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H12" s="1">
-        <v>0.725</v>
+        <v>0.7045454545454546</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
@@ -2503,16 +2503,16 @@
         <v>4</v>
       </c>
       <c r="M12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N12" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O12" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -2520,28 +2520,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2332</v>
+        <v>2605</v>
       </c>
       <c r="C13" s="1">
-        <v>58.3</v>
+        <v>59.20454545454545</v>
       </c>
       <c r="D13" s="1">
-        <v>374</v>
+        <v>403</v>
       </c>
       <c r="E13" s="1">
-        <v>9.35</v>
+        <v>9.159090909090908</v>
       </c>
       <c r="F13" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1">
-        <v>0.65</v>
+        <v>0.6590909090909091</v>
       </c>
       <c r="I13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="1">
         <v>2</v>
@@ -2550,16 +2550,16 @@
         <v>2</v>
       </c>
       <c r="L13" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M13" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N13" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="O13" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P13" s="1">
         <v>3</v>
@@ -2570,46 +2570,46 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>2285</v>
+        <v>2517</v>
       </c>
       <c r="C14" s="1">
-        <v>57.125</v>
+        <v>57.20454545454545</v>
       </c>
       <c r="D14" s="1">
-        <v>392</v>
+        <v>429</v>
       </c>
       <c r="E14" s="1">
-        <v>9.8</v>
+        <v>9.75</v>
       </c>
       <c r="F14" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G14" s="1">
+        <v>44</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1">
+        <v>12</v>
+      </c>
+      <c r="N14" s="1">
+        <v>19</v>
+      </c>
+      <c r="O14" s="1">
         <v>40</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>3</v>
-      </c>
-      <c r="K14" s="1">
-        <v>2</v>
-      </c>
-      <c r="L14" s="1">
-        <v>5</v>
-      </c>
-      <c r="M14" s="1">
-        <v>11</v>
-      </c>
-      <c r="N14" s="1">
-        <v>18</v>
-      </c>
-      <c r="O14" s="1">
-        <v>36</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
@@ -2620,28 +2620,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2173</v>
+        <v>2479</v>
       </c>
       <c r="C15" s="1">
-        <v>54.325</v>
+        <v>56.34090909090909</v>
       </c>
       <c r="D15" s="1">
-        <v>405</v>
+        <v>432</v>
       </c>
       <c r="E15" s="1">
-        <v>10.125</v>
+        <v>9.818181818181818</v>
       </c>
       <c r="F15" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H15" s="1">
-        <v>0.6</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="I15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J15" s="1">
         <v>4</v>
@@ -2650,16 +2650,16 @@
         <v>2</v>
       </c>
       <c r="L15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N15" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O15" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P15" s="1">
         <v>5</v>
@@ -2670,46 +2670,46 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>2191</v>
+        <v>2424</v>
       </c>
       <c r="C16" s="1">
-        <v>59.21621621621622</v>
+        <v>59.1219512195122</v>
       </c>
       <c r="D16" s="1">
-        <v>342</v>
+        <v>376</v>
       </c>
       <c r="E16" s="1">
-        <v>9.243243243243244</v>
+        <v>9.170731707317072</v>
       </c>
       <c r="F16" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1">
-        <v>0.6756756756756757</v>
+        <v>0.6829268292682927</v>
       </c>
       <c r="I16" s="1">
         <v>3</v>
       </c>
       <c r="J16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="1">
         <v>2</v>
       </c>
       <c r="L16" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N16" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="O16" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P16" s="1">
         <v>2</v>
@@ -2720,25 +2720,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>2331</v>
+        <v>2514</v>
       </c>
       <c r="C17" s="1">
-        <v>61.3421052631579</v>
+        <v>61.31707317073171</v>
       </c>
       <c r="D17" s="1">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="E17" s="1">
-        <v>9.052631578947368</v>
+        <v>8.951219512195122</v>
       </c>
       <c r="F17" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G17" s="1">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H17" s="1">
-        <v>0.7631578947368421</v>
+        <v>0.7560975609756098</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -2753,13 +2753,13 @@
         <v>5</v>
       </c>
       <c r="M17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N17" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O17" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
@@ -2770,25 +2770,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1499</v>
+        <v>1533</v>
       </c>
       <c r="C18" s="1">
-        <v>51.689655172413794</v>
+        <v>51.1</v>
       </c>
       <c r="D18" s="1">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="E18" s="1">
-        <v>11.137931034482758</v>
+        <v>11.266666666666667</v>
       </c>
       <c r="F18" s="1">
         <v>16</v>
       </c>
       <c r="G18" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H18" s="1">
-        <v>0.5517241379310345</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
@@ -2809,7 +2809,7 @@
         <v>14</v>
       </c>
       <c r="O18" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P18" s="1">
         <v>2</v>
@@ -3020,25 +3020,25 @@
         <v>-1</v>
       </c>
       <c r="B23" s="1">
-        <v>2246</v>
+        <v>2418</v>
       </c>
       <c r="C23" s="1">
-        <v>59.10526315789474</v>
+        <v>57.57142857142857</v>
       </c>
       <c r="D23" s="1">
-        <v>372</v>
+        <v>419</v>
       </c>
       <c r="E23" s="1">
-        <v>9.789473684210526</v>
+        <v>9.976190476190476</v>
       </c>
       <c r="F23" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G23" s="1">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H23" s="1">
-        <v>0.6578947368421053</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
@@ -3056,10 +3056,10 @@
         <v>11</v>
       </c>
       <c r="N23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O23" s="1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="P23" s="1">
         <v>1</v>
@@ -3070,46 +3070,46 @@
         <v>-2</v>
       </c>
       <c r="B24" s="1">
-        <v>2392</v>
+        <v>2675</v>
       </c>
       <c r="C24" s="1">
-        <v>59.8</v>
+        <v>60.79545454545455</v>
       </c>
       <c r="D24" s="1">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="E24" s="1">
-        <v>9.275</v>
+        <v>9.022727272727273</v>
       </c>
       <c r="F24" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G24" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H24" s="1">
-        <v>0.75</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24" s="1">
         <v>1</v>
       </c>
       <c r="L24" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M24" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N24" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O24" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -3120,28 +3120,28 @@
         <v>-3</v>
       </c>
       <c r="B25" s="1">
-        <v>2169</v>
+        <v>2466</v>
       </c>
       <c r="C25" s="1">
-        <v>54.225</v>
+        <v>56.04545454545455</v>
       </c>
       <c r="D25" s="1">
-        <v>406</v>
+        <v>435</v>
       </c>
       <c r="E25" s="1">
-        <v>10.15</v>
+        <v>9.886363636363637</v>
       </c>
       <c r="F25" s="1">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G25" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H25" s="1">
-        <v>0.575</v>
+        <v>0.6136363636363636</v>
       </c>
       <c r="I25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" s="1">
         <v>3</v>
@@ -3150,16 +3150,16 @@
         <v>3</v>
       </c>
       <c r="L25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M25" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N25" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="O25" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P25" s="1">
         <v>4</v>
@@ -3170,25 +3170,25 @@
         <v>-4</v>
       </c>
       <c r="B26" s="1">
-        <v>2419</v>
+        <v>2629</v>
       </c>
       <c r="C26" s="1">
-        <v>62.02564102564103</v>
+        <v>61.13953488372093</v>
       </c>
       <c r="D26" s="1">
-        <v>332</v>
+        <v>371</v>
       </c>
       <c r="E26" s="1">
-        <v>8.512820512820513</v>
+        <v>8.627906976744185</v>
       </c>
       <c r="F26" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G26" s="1">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H26" s="1">
-        <v>0.7948717948717948</v>
+        <v>0.813953488372093</v>
       </c>
       <c r="I26" s="1">
         <v>2</v>
@@ -3206,10 +3206,10 @@
         <v>12</v>
       </c>
       <c r="N26" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O26" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P26" s="1">
         <v>2</v>
@@ -3220,49 +3220,49 @@
         <v>-5</v>
       </c>
       <c r="B27" s="1">
-        <v>2183</v>
+        <v>2459</v>
       </c>
       <c r="C27" s="1">
-        <v>54.575</v>
+        <v>55.88636363636363</v>
       </c>
       <c r="D27" s="1">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="E27" s="1">
-        <v>10.1</v>
+        <v>9.75</v>
       </c>
       <c r="F27" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G27" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H27" s="1">
-        <v>0.625</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="I27" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="1">
         <v>1</v>
       </c>
       <c r="L27" s="1">
+        <v>6</v>
+      </c>
+      <c r="M27" s="1">
+        <v>9</v>
+      </c>
+      <c r="N27" s="1">
+        <v>24</v>
+      </c>
+      <c r="O27" s="1">
+        <v>39</v>
+      </c>
+      <c r="P27" s="1">
         <v>4</v>
-      </c>
-      <c r="M27" s="1">
-        <v>7</v>
-      </c>
-      <c r="N27" s="1">
-        <v>21</v>
-      </c>
-      <c r="O27" s="1">
-        <v>35</v>
-      </c>
-      <c r="P27" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -3270,25 +3270,25 @@
         <v>-6</v>
       </c>
       <c r="B28" s="1">
-        <v>2237</v>
+        <v>2447</v>
       </c>
       <c r="C28" s="1">
-        <v>55.925</v>
+        <v>55.61363636363637</v>
       </c>
       <c r="D28" s="1">
-        <v>407</v>
+        <v>445</v>
       </c>
       <c r="E28" s="1">
-        <v>10.175</v>
+        <v>10.113636363636363</v>
       </c>
       <c r="F28" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G28" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H28" s="1">
-        <v>0.625</v>
+        <v>0.6136363636363636</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
@@ -3303,13 +3303,13 @@
         <v>4</v>
       </c>
       <c r="M28" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N28" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O28" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P28" s="1">
         <v>3</v>
@@ -3320,25 +3320,25 @@
         <v>-7</v>
       </c>
       <c r="B29" s="1">
-        <v>2394</v>
+        <v>2565</v>
       </c>
       <c r="C29" s="1">
-        <v>59.85</v>
+        <v>58.29545454545455</v>
       </c>
       <c r="D29" s="1">
-        <v>346</v>
+        <v>391</v>
       </c>
       <c r="E29" s="1">
-        <v>8.65</v>
+        <v>8.886363636363637</v>
       </c>
       <c r="F29" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G29" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H29" s="1">
-        <v>0.65</v>
+        <v>0.6590909090909091</v>
       </c>
       <c r="I29" s="1">
         <v>2</v>
@@ -3356,10 +3356,10 @@
         <v>18</v>
       </c>
       <c r="N29" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O29" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P29" s="1">
         <v>2</v>
@@ -3370,25 +3370,25 @@
         <v>-8</v>
       </c>
       <c r="B30" s="1">
-        <v>2321</v>
+        <v>2603</v>
       </c>
       <c r="C30" s="1">
-        <v>58.025</v>
+        <v>59.15909090909091</v>
       </c>
       <c r="D30" s="1">
-        <v>374</v>
+        <v>398</v>
       </c>
       <c r="E30" s="1">
-        <v>9.35</v>
+        <v>9.045454545454545</v>
       </c>
       <c r="F30" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G30" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H30" s="1">
-        <v>0.675</v>
+        <v>0.7045454545454546</v>
       </c>
       <c r="I30" s="1">
         <v>3</v>
@@ -3397,19 +3397,19 @@
         <v>2</v>
       </c>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L30" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M30" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N30" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O30" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="P30" s="1">
         <v>5</v>
@@ -3420,25 +3420,25 @@
         <v>-9</v>
       </c>
       <c r="B31" s="1">
-        <v>2475</v>
+        <v>2692</v>
       </c>
       <c r="C31" s="1">
-        <v>61.875</v>
+        <v>61.18181818181818</v>
       </c>
       <c r="D31" s="1">
-        <v>353</v>
+        <v>391</v>
       </c>
       <c r="E31" s="1">
-        <v>8.825</v>
+        <v>8.886363636363637</v>
       </c>
       <c r="F31" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G31" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H31" s="1">
-        <v>0.725</v>
+        <v>0.7045454545454546</v>
       </c>
       <c r="I31" s="1">
         <v>2</v>
@@ -3453,13 +3453,13 @@
         <v>8</v>
       </c>
       <c r="M31" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N31" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O31" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="P31" s="1">
         <v>0</v>
@@ -3470,46 +3470,46 @@
         <v>-10</v>
       </c>
       <c r="B32" s="1">
-        <v>2247</v>
+        <v>2517</v>
       </c>
       <c r="C32" s="1">
-        <v>56.175</v>
+        <v>58.53488372093023</v>
       </c>
       <c r="D32" s="1">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="E32" s="1">
-        <v>9.7</v>
+        <v>9.255813953488373</v>
       </c>
       <c r="F32" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G32" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H32" s="1">
-        <v>0.7</v>
+        <v>0.7209302325581395</v>
       </c>
       <c r="I32" s="1">
+        <v>4</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
         <v>3</v>
       </c>
-      <c r="J32" s="1">
-        <v>0</v>
-      </c>
-      <c r="K32" s="1">
-        <v>2</v>
-      </c>
       <c r="L32" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M32" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N32" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O32" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="P32" s="1">
         <v>2</v>
@@ -3520,25 +3520,25 @@
         <v>-11</v>
       </c>
       <c r="B33" s="1">
-        <v>2278</v>
+        <v>2485</v>
       </c>
       <c r="C33" s="1">
-        <v>56.95</v>
+        <v>56.47727272727273</v>
       </c>
       <c r="D33" s="1">
-        <v>390</v>
+        <v>432</v>
       </c>
       <c r="E33" s="1">
-        <v>9.75</v>
+        <v>9.818181818181818</v>
       </c>
       <c r="F33" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G33" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H33" s="1">
-        <v>0.675</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
@@ -3553,13 +3553,13 @@
         <v>6</v>
       </c>
       <c r="M33" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N33" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O33" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P33" s="1">
         <v>4</v>
@@ -3570,25 +3570,25 @@
         <v>-12</v>
       </c>
       <c r="B34" s="1">
-        <v>2508</v>
+        <v>2634</v>
       </c>
       <c r="C34" s="1">
-        <v>62.7</v>
+        <v>61.25581395348837</v>
       </c>
       <c r="D34" s="1">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="E34" s="1">
-        <v>8.675</v>
+        <v>8.837209302325581</v>
       </c>
       <c r="F34" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G34" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H34" s="1">
-        <v>0.725</v>
+        <v>0.7209302325581395</v>
       </c>
       <c r="I34" s="1">
         <v>4</v>
@@ -3606,13 +3606,13 @@
         <v>13</v>
       </c>
       <c r="N34" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O34" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P34" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -3620,46 +3620,46 @@
         <v>-13</v>
       </c>
       <c r="B35" s="1">
-        <v>2313</v>
+        <v>2658</v>
       </c>
       <c r="C35" s="1">
-        <v>57.825</v>
+        <v>60.40909090909091</v>
       </c>
       <c r="D35" s="1">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="E35" s="1">
-        <v>9.4</v>
+        <v>8.795454545454545</v>
       </c>
       <c r="F35" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H35" s="1">
-        <v>0.65</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="I35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K35" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L35" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M35" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N35" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O35" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P35" s="1">
         <v>3</v>
@@ -3670,25 +3670,25 @@
         <v>-14</v>
       </c>
       <c r="B36" s="1">
-        <v>2558</v>
+        <v>2719</v>
       </c>
       <c r="C36" s="1">
-        <v>63.95</v>
+        <v>61.79545454545455</v>
       </c>
       <c r="D36" s="1">
-        <v>336</v>
+        <v>386</v>
       </c>
       <c r="E36" s="1">
-        <v>8.4</v>
+        <v>8.772727272727273</v>
       </c>
       <c r="F36" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G36" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H36" s="1">
-        <v>0.675</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="I36" s="1">
         <v>5</v>
@@ -3706,10 +3706,10 @@
         <v>13</v>
       </c>
       <c r="N36" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O36" s="1">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>
@@ -3720,46 +3720,46 @@
         <v>-15</v>
       </c>
       <c r="B37" s="1">
-        <v>2254</v>
+        <v>2528</v>
       </c>
       <c r="C37" s="1">
-        <v>59.31578947368421</v>
+        <v>60.19047619047619</v>
       </c>
       <c r="D37" s="1">
-        <v>350</v>
+        <v>377</v>
       </c>
       <c r="E37" s="1">
-        <v>9.210526315789474</v>
+        <v>8.976190476190476</v>
       </c>
       <c r="F37" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G37" s="1">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H37" s="1">
-        <v>0.7368421052631579</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="I37" s="1">
         <v>3</v>
       </c>
       <c r="J37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37" s="1">
         <v>2</v>
       </c>
       <c r="L37" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N37" s="1">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O37" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P37" s="1">
         <v>3</v>
@@ -3770,25 +3770,25 @@
         <v>-16</v>
       </c>
       <c r="B38" s="1">
-        <v>2409</v>
+        <v>2610</v>
       </c>
       <c r="C38" s="1">
-        <v>63.39473684210526</v>
+        <v>63.65853658536585</v>
       </c>
       <c r="D38" s="1">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="E38" s="1">
-        <v>8.710526315789474</v>
+        <v>8.609756097560975</v>
       </c>
       <c r="F38" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G38" s="1">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H38" s="1">
-        <v>0.7105263157894737</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="I38" s="1">
         <v>3</v>
@@ -3803,13 +3803,13 @@
         <v>9</v>
       </c>
       <c r="M38" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N38" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O38" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="P38" s="1">
         <v>1</v>
@@ -3820,25 +3820,25 @@
         <v>-17</v>
       </c>
       <c r="B39" s="1">
-        <v>1857</v>
+        <v>1931</v>
       </c>
       <c r="C39" s="1">
-        <v>61.9</v>
+        <v>62.29032258064516</v>
       </c>
       <c r="D39" s="1">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="E39" s="1">
-        <v>8.7</v>
+        <v>8.612903225806452</v>
       </c>
       <c r="F39" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G39" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H39" s="1">
-        <v>0.8333333333333334</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="I39" s="1">
         <v>1</v>
@@ -3856,10 +3856,10 @@
         <v>8</v>
       </c>
       <c r="N39" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O39" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P39" s="1">
         <v>1</v>

</xml_diff>